<commit_message>
update: modify errors from the draft
</commit_message>
<xml_diff>
--- a/WPCN/for_final_paper.xlsx
+++ b/WPCN/for_final_paper.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="30">
   <si>
     <t>Problem/Size</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -361,14 +361,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CT.RATE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CT.RATE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CT.AVERAGE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -382,6 +374,10 @@
   </si>
   <si>
     <t>CT.AVGMAX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CT.RATE (%)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -700,6 +696,30 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -712,47 +732,23 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1042,7 +1038,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1054,32 +1050,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="F1" s="18" t="s">
+      <c r="D1" s="16"/>
+      <c r="F1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="18"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="F2" s="13" t="s">
+      <c r="D2" s="15"/>
+      <c r="F2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="1">
         <v>6</v>
       </c>
@@ -1094,7 +1090,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1116,7 +1112,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="16"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1136,7 +1132,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="16"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1156,7 +1152,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="16"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1176,7 +1172,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="16"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1196,7 +1192,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="17"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1212,36 +1208,36 @@
       </c>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>5.5150370999999994E-4</v>
+        <v>5.2549784399999998E-4</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="F11" s="18" t="s">
+      <c r="D11" s="16"/>
+      <c r="F11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="18"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="13" t="s">
+      <c r="B12" s="18"/>
+      <c r="C12" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="F12" s="13" t="s">
+      <c r="D12" s="15"/>
+      <c r="F12" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="14"/>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="1">
         <v>6</v>
       </c>
@@ -1256,7 +1252,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1278,7 +1274,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="16"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
@@ -1298,7 +1294,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="16"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
@@ -1318,7 +1314,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="16"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
@@ -1338,7 +1334,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="16"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
@@ -1358,7 +1354,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="17"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1374,28 +1370,28 @@
       </c>
       <c r="G19" s="3">
         <f t="shared" si="2"/>
-        <v>5.2905682499999993E-4</v>
+        <v>5.0410943E-4</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F21" s="19" t="s">
+      <c r="F21" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="19"/>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="F22" s="13" t="s">
+      <c r="B22" s="18"/>
+      <c r="F22" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="14"/>
+      <c r="G22" s="15"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
       <c r="F23" s="1">
         <v>6</v>
       </c>
@@ -1404,7 +1400,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1418,7 +1414,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" s="16"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
@@ -1430,7 +1426,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="16"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
@@ -1442,7 +1438,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="16"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
@@ -1454,7 +1450,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A28" s="16"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
@@ -1466,7 +1462,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" s="17"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
@@ -1474,28 +1470,28 @@
         <v>9.9400000000000009E-4</v>
       </c>
       <c r="G29" s="2">
-        <v>6.1499999999999999E-4</v>
+        <v>5.8600000000000004E-4</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F31" s="18" t="s">
+      <c r="F31" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="18"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="10"/>
-      <c r="F32" s="13" t="s">
+      <c r="B32" s="18"/>
+      <c r="F32" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G32" s="14"/>
+      <c r="G32" s="15"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" s="11"/>
-      <c r="B33" s="12"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="20"/>
       <c r="F33" s="1">
         <v>6</v>
       </c>
@@ -1504,7 +1500,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1520,7 +1516,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A35" s="16"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
@@ -1534,7 +1530,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A36" s="16"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="1" t="s">
         <v>4</v>
       </c>
@@ -1548,7 +1544,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="16"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="1" t="s">
         <v>5</v>
       </c>
@@ -1562,7 +1558,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A38" s="16"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="1" t="s">
         <v>6</v>
       </c>
@@ -1576,7 +1572,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A39" s="17"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
@@ -1591,6 +1587,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A32:B33"/>
     <mergeCell ref="A34:A39"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="F32:G32"/>
@@ -1607,10 +1607,6 @@
     <mergeCell ref="A4:A9"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A2:B3"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="A32:B33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1622,42 +1618,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="25"/>
+    <col min="1" max="1" width="8.6640625" style="9"/>
     <col min="2" max="3" width="14.25" customWidth="1"/>
     <col min="4" max="7" width="11.58203125" customWidth="1"/>
-    <col min="8" max="11" width="8.6640625" style="25"/>
+    <col min="8" max="11" width="8.6640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="25" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="D2" s="26" t="s">
+    <row r="1" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="26"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="2:7" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="23" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="23" t="s">
+      <c r="E3" s="23"/>
+      <c r="F3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="24"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4" s="7" t="s">
@@ -1680,7 +1676,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -1702,7 +1698,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B6" s="21"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1722,7 +1718,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B7" s="22"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="5" t="s">
         <v>24</v>
       </c>
@@ -1738,33 +1734,33 @@
       </c>
       <c r="G7" s="4">
         <f t="shared" si="0"/>
-        <v>5.5150370999999994E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" s="25" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="9" spans="2:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="D9" s="26" t="s">
+        <v>5.2549784399999998E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" s="9" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="9" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D9" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="26"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="2:7" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="23" t="s">
+      <c r="C10" s="26"/>
+      <c r="D10" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="23" t="s">
+      <c r="E10" s="23"/>
+      <c r="F10" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="24"/>
+      <c r="G10" s="23"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B11" s="7" t="s">
@@ -1787,7 +1783,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1809,7 +1805,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B13" s="21"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="5" t="s">
         <v>23</v>
       </c>
@@ -1829,7 +1825,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B14" s="22"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="5" t="s">
         <v>24</v>
       </c>
@@ -1845,29 +1841,29 @@
       </c>
       <c r="G14" s="4">
         <f t="shared" si="1"/>
-        <v>5.2905682499999993E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" s="25" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="16" spans="2:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="F16" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="26"/>
+        <v>5.0410943E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F16" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="21"/>
     </row>
     <row r="17" spans="2:7" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="23" t="s">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="24"/>
+      <c r="G17" s="23"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="7" t="s">
         <v>19</v>
       </c>
@@ -1882,9 +1878,9 @@
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="21" t="s">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="24" t="s">
         <v>21</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -1898,9 +1894,9 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="21"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="24"/>
       <c r="E20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1912,9 +1908,9 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="22"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="25"/>
       <c r="E21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1922,29 +1918,29 @@
         <v>9.9400000000000009E-4</v>
       </c>
       <c r="G21" s="8">
-        <v>6.1499999999999999E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" s="25" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="23" spans="2:7" s="25" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="F23" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" s="26"/>
+        <v>5.8600000000000004E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="23" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="F23" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="2:7" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="23" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="G24" s="24"/>
+      <c r="G24" s="23"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="7" t="s">
         <v>19</v>
       </c>
@@ -1959,9 +1955,9 @@
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="21" t="s">
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="24" t="s">
         <v>21</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -1977,9 +1973,9 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="21"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="24"/>
       <c r="E27" s="5" t="s">
         <v>23</v>
       </c>
@@ -1993,9 +1989,9 @@
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="22"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="5" t="s">
         <v>24</v>
       </c>
@@ -2008,18 +2004,17 @@
         <v>1.0424281172443055</v>
       </c>
     </row>
-    <row r="29" spans="2:7" s="25" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="30" spans="2:7" s="25" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="31" spans="2:7" s="25" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="32" spans="2:7" s="25" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="29" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="30" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="31" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="32" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="B12:B14"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="D26:D28"/>
@@ -2027,15 +2022,16 @@
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="F24:G24"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F5:G7">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2048,36 +2044,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:E7">
-    <cfRule type="dataBar" priority="7">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="0" tint="-0.14999847407452621"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{021104DF-CF7E-4FDF-884A-AF90A133E3C7}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12:E14">
-    <cfRule type="dataBar" priority="8">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="0" tint="-0.14999847407452621"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B1C5AFE8-2A9C-4052-8265-ECE0505385B5}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F12:G14">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2091,7 +2059,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:G21">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2105,7 +2073,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26:G28">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2114,6 +2082,34 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{D9E48C72-BD84-4ED8-B42A-EDBABE80D1AC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:E7 D12:E14">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="100"/>
+        <color theme="0" tint="-0.14999847407452621"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B20C883A-ED20-4860-97C5-E46DDF87EC6B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:G7 F12:G14">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color theme="2" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{45EFABD3-AF6A-43DD-B61A-4E2BCCD88CE0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2133,28 +2129,6 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>F5:G7</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{021104DF-CF7E-4FDF-884A-AF90A133E3C7}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="min"/>
-              <x14:cfvo type="max"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D5:E7</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B1C5AFE8-2A9C-4052-8265-ECE0505385B5}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="min"/>
-              <x14:cfvo type="max"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D12:E14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6A732025-1111-494D-8710-A546F731D4A8}">
@@ -2189,6 +2163,34 @@
           </x14:cfRule>
           <xm:sqref>F26:G28</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B20C883A-ED20-4860-97C5-E46DDF87EC6B}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>100</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D5:E7 D12:E14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{45EFABD3-AF6A-43DD-B61A-4E2BCCD88CE0}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="max"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F5:G7 F12:G14</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
update: add comparison graph (Figure 9)
</commit_message>
<xml_diff>
--- a/WPCN/for_final_paper.xlsx
+++ b/WPCN/for_final_paper.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
   <si>
     <t>Problem/Size</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -380,6 +380,38 @@
     <t>Size / WDs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Our Method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Original Paper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8x8 / 6 WDs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12x12 / 6 WDs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16x16 / 6 WDs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8x8 / 10 WDs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12x12 / 10 WDs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16x16 / 10 WDs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -389,7 +421,7 @@
     <numFmt numFmtId="176" formatCode="0.000000_ "/>
     <numFmt numFmtId="177" formatCode="0.0000_ "/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,6 +511,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -683,7 +731,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -714,53 +762,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -779,6 +782,69 @@
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3415,6 +3481,453 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:t>CT.RATE (%) of</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
+              <a:t> our method vs. the methodology in original paper</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="ko-KR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'for paper'!$D$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Our Method</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'for paper'!$C$27:$C$32</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8x8 / 6 WDs</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12x12 / 6 WDs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16x16 / 6 WDs</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8x8 / 10 WDs</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12x12 / 10 WDs</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16x16 / 10 WDs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'for paper'!$D$27:$D$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000_ </c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>93.847700000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>88.978200000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80.031800000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98.628299999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.173500000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89.675399999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2F19-4BCA-8094-7E8AD85B1A8D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'for paper'!$E$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Original Paper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'for paper'!$C$27:$C$32</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8x8 / 6 WDs</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12x12 / 6 WDs</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16x16 / 6 WDs</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8x8 / 10 WDs</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12x12 / 10 WDs</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16x16 / 10 WDs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'for paper'!$E$27:$E$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000_ </c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40.138599999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.0471</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.801500000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54.5807</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76.190200000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>86.025499999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2F19-4BCA-8094-7E8AD85B1A8D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1679866800"/>
+        <c:axId val="1679869296"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1679866800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1679869296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1679869296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="30"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0_ " sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1679866800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3655,6 +4168,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -6172,6 +6725,509 @@
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6855,6 +7911,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7136,32 +8222,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="F1" s="19" t="s">
+      <c r="D1" s="27"/>
+      <c r="F1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="19"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="14" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="F2" s="14" t="s">
+      <c r="D2" s="21"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="15"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="1">
         <v>6</v>
       </c>
@@ -7176,7 +8262,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -7198,7 +8284,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="17"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -7218,7 +8304,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="17"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -7238,7 +8324,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="17"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -7258,7 +8344,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="17"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -7278,7 +8364,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="18"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -7298,32 +8384,32 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="F11" s="19" t="s">
+      <c r="D11" s="27"/>
+      <c r="F11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="19"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="14" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="F12" s="14" t="s">
+      <c r="D12" s="21"/>
+      <c r="F12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="21"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="1">
         <v>6</v>
       </c>
@@ -7338,7 +8424,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -7360,7 +8446,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="17"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
@@ -7380,7 +8466,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="17"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
@@ -7400,7 +8486,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="17"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
@@ -7420,7 +8506,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="17"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
@@ -7440,7 +8526,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="18"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
@@ -7460,24 +8546,24 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="20"/>
+      <c r="G21" s="27"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="F22" s="14" t="s">
+      <c r="B22" s="23"/>
+      <c r="F22" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="15"/>
+      <c r="G22" s="21"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="25"/>
       <c r="F23" s="1">
         <v>6</v>
       </c>
@@ -7486,7 +8572,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -7500,7 +8586,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" s="17"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
@@ -7512,7 +8598,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="17"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
@@ -7524,7 +8610,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="17"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
@@ -7536,7 +8622,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A28" s="17"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
@@ -7548,7 +8634,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" s="18"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
@@ -7560,24 +8646,24 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="19"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="F32" s="14" t="s">
+      <c r="B32" s="23"/>
+      <c r="F32" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G32" s="15"/>
+      <c r="G32" s="21"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" s="12"/>
-      <c r="B33" s="13"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="25"/>
       <c r="F33" s="1">
         <v>6</v>
       </c>
@@ -7586,7 +8672,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -7602,7 +8688,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A35" s="17"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
@@ -7616,7 +8702,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A36" s="17"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="1" t="s">
         <v>4</v>
       </c>
@@ -7630,7 +8716,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="17"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="1" t="s">
         <v>5</v>
       </c>
@@ -7644,7 +8730,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A38" s="17"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="1" t="s">
         <v>6</v>
       </c>
@@ -7658,7 +8744,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A39" s="18"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
@@ -7673,26 +8759,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="C12:D12"/>
     <mergeCell ref="A4:A9"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="F32:G32"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F21:G21"/>
     <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F12:G12"/>
     <mergeCell ref="A12:B13"/>
-    <mergeCell ref="C12:D12"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A32:B33"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="A22:B23"/>
-    <mergeCell ref="A24:A29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7702,10 +8788,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -7718,18 +8804,18 @@
   <sheetData>
     <row r="1" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="21" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21" t="s">
+      <c r="E2" s="28"/>
+      <c r="F2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="21"/>
+      <c r="G2" s="28"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" s="9"/>
@@ -7739,10 +8825,10 @@
       <c r="D3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="13" t="s">
         <v>27</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -7750,7 +8836,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="29" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -7759,72 +8845,72 @@
       <c r="D4" s="6">
         <v>93.847700000000003</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="16">
         <v>98.628299999999996</v>
       </c>
-      <c r="F4" s="29">
-        <f>F16*D4/100</f>
+      <c r="F4" s="14">
+        <f t="shared" ref="F4:G6" si="0">F16*D4/100</f>
         <v>1.0174967634E-2</v>
       </c>
       <c r="G4" s="4">
-        <f>G16*E4/100</f>
+        <f t="shared" si="0"/>
         <v>6.7570248330000001E-3</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B5" s="25"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="6">
         <v>88.978200000000001</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="16">
         <v>91.173500000000004</v>
       </c>
-      <c r="F5" s="29">
-        <f>F17*D5/100</f>
+      <c r="F5" s="14">
+        <f t="shared" si="0"/>
         <v>2.6257466820000003E-3</v>
       </c>
       <c r="G5" s="4">
-        <f>G17*E5/100</f>
+        <f t="shared" si="0"/>
         <v>1.6310939150000002E-3</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B6" s="25"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="6">
         <v>80.031800000000004</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="16">
         <v>89.675399999999996</v>
       </c>
-      <c r="F6" s="29">
-        <f>F18*D6/100</f>
+      <c r="F6" s="14">
+        <f t="shared" si="0"/>
         <v>7.9551609200000008E-4</v>
       </c>
       <c r="G6" s="4">
-        <f>G18*E6/100</f>
+        <f t="shared" si="0"/>
         <v>5.2549784399999998E-4</v>
       </c>
     </row>
     <row r="7" spans="2:7" s="9" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="8" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="21" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21" t="s">
+      <c r="E8" s="28"/>
+      <c r="F8" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="21"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B9" s="9"/>
@@ -7834,10 +8920,10 @@
       <c r="D9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="13" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="5" t="s">
@@ -7845,7 +8931,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="29" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -7854,55 +8940,55 @@
       <c r="D10" s="6">
         <v>40.138599999999997</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="16">
         <v>54.5807</v>
       </c>
-      <c r="F10" s="29">
-        <f>F16*D10/100</f>
+      <c r="F10" s="14">
+        <f t="shared" ref="F10:G12" si="1">F16*D10/100</f>
         <v>4.351827011999999E-3</v>
       </c>
       <c r="G10" s="4">
-        <f>G16*E10/100</f>
+        <f t="shared" si="1"/>
         <v>3.7393237570000006E-3</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B11" s="25"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="6">
         <v>72.0471</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="16">
         <v>76.190200000000004</v>
       </c>
-      <c r="F11" s="29">
-        <f>F17*D11/100</f>
+      <c r="F11" s="14">
+        <f t="shared" si="1"/>
         <v>2.1261099209999999E-3</v>
       </c>
       <c r="G11" s="4">
-        <f>G17*E11/100</f>
+        <f t="shared" si="1"/>
         <v>1.3630426780000002E-3</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B12" s="25"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="6">
         <v>90.801500000000004</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="16">
         <v>86.025499999999994</v>
       </c>
-      <c r="F12" s="29">
-        <f>F18*D12/100</f>
+      <c r="F12" s="14">
+        <f t="shared" si="1"/>
         <v>9.025669100000001E-4</v>
       </c>
       <c r="G12" s="4">
-        <f>G18*E12/100</f>
+        <f t="shared" si="1"/>
         <v>5.0410943E-4</v>
       </c>
     </row>
@@ -7910,17 +8996,17 @@
     <row r="14" spans="2:7" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="23" t="s">
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="23"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="24"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="7" t="s">
         <v>29</v>
       </c>
@@ -7934,7 +9020,7 @@
     <row r="16" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="29" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -7950,7 +9036,7 @@
     <row r="17" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="25"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="5" t="s">
         <v>20</v>
       </c>
@@ -7964,7 +9050,7 @@
     <row r="18" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="25"/>
+      <c r="D18" s="29"/>
       <c r="E18" s="5" t="s">
         <v>21</v>
       </c>
@@ -7979,12 +9065,12 @@
     <row r="20" spans="2:7" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="21" t="s">
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="21"/>
+      <c r="G20" s="28"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B21" s="9"/>
@@ -8003,69 +9089,194 @@
     <row r="22" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="29" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F22" s="4">
-        <f>F4/F10</f>
+        <f t="shared" ref="F22:G24" si="2">F4/F10</f>
         <v>2.3380910146342928</v>
       </c>
       <c r="G22" s="4">
-        <f>G4/G10</f>
+        <f t="shared" si="2"/>
         <v>1.8070178652893787</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="25"/>
+      <c r="D23" s="29"/>
       <c r="E23" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F23" s="4">
-        <f>F5/F11</f>
+        <f t="shared" si="2"/>
         <v>1.2350004372139893</v>
       </c>
       <c r="G23" s="4">
-        <f>G5/G11</f>
+        <f t="shared" si="2"/>
         <v>1.1966565253799044</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="25"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F24" s="4">
-        <f>F6/F12</f>
+        <f t="shared" si="2"/>
         <v>0.88139292853091633</v>
       </c>
       <c r="G24" s="4">
-        <f>G6/G12</f>
+        <f t="shared" si="2"/>
         <v>1.0424281172443055</v>
       </c>
     </row>
     <row r="25" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="26" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="27" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="28" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C26" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" s="9" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="34">
+        <f>D4</f>
+        <v>93.847700000000003</v>
+      </c>
+      <c r="E27" s="34">
+        <f>D10</f>
+        <v>40.138599999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="37"/>
+      <c r="C28" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="34">
+        <f>D5</f>
+        <v>88.978200000000001</v>
+      </c>
+      <c r="E28" s="34">
+        <f>D11</f>
+        <v>72.0471</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B29" s="37"/>
+      <c r="C29" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="34">
+        <f>D6</f>
+        <v>80.031800000000004</v>
+      </c>
+      <c r="E29" s="34">
+        <f>D12</f>
+        <v>90.801500000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B30" s="37"/>
+      <c r="C30" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="34">
+        <f>E4</f>
+        <v>98.628299999999996</v>
+      </c>
+      <c r="E30" s="34">
+        <f>E10</f>
+        <v>54.5807</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B31" s="37"/>
+      <c r="C31" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="34">
+        <f>E5</f>
+        <v>91.173500000000004</v>
+      </c>
+      <c r="E31" s="34">
+        <f>E11</f>
+        <v>76.190200000000004</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B32" s="37"/>
+      <c r="C32" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="34">
+        <f>E6</f>
+        <v>89.675399999999996</v>
+      </c>
+      <c r="E32" s="34">
+        <f>E12</f>
+        <v>86.025499999999994</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D16:D18"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="B8:C8"/>
   </mergeCells>

</xml_diff>

<commit_message>
add: update paper (applied the issue)
</commit_message>
<xml_diff>
--- a/WPCN/for_final_paper.xlsx
+++ b/WPCN/for_final_paper.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19690" windowHeight="9910" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (old version)" sheetId="1" r:id="rId1"/>
     <sheet name="for paper" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="38">
   <si>
     <t>Problem/Size</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -421,7 +421,7 @@
     <numFmt numFmtId="176" formatCode="0.000000_ "/>
     <numFmt numFmtId="177" formatCode="0.0000_ "/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,8 +532,24 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -567,6 +583,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -731,7 +753,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -750,14 +772,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
@@ -780,7 +796,31 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -816,35 +856,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1878,13 +1921,13 @@
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>40.138599999999997</c:v>
+                  <c:v>65.5779</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>72.0471</c:v>
+                  <c:v>89.167599999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90.801500000000004</c:v>
+                  <c:v>100.65649999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1958,13 +2001,13 @@
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>54.5807</c:v>
+                  <c:v>71.962699999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76.190200000000004</c:v>
+                  <c:v>90.393100000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>86.025499999999994</c:v>
+                  <c:v>96.860600000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2044,7 +2087,7 @@
         <c:axId val="1574848687"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="40"/>
+          <c:min val="65"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2317,13 +2360,13 @@
                 <c:formatCode>0.000000_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.351827011999999E-3</c:v>
+                  <c:v>7.1099559179999992E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1261099209999999E-3</c:v>
+                  <c:v>2.6313358759999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.025669100000001E-4</c:v>
+                  <c:v>1.0005256099999999E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2397,13 +2440,13 @@
                 <c:formatCode>0.000000_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.7393237570000006E-3</c:v>
+                  <c:v>4.9301645770000006E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3630426780000002E-3</c:v>
+                  <c:v>1.6171325590000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0410943E-4</c:v>
+                  <c:v>5.6760311600000004E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2483,7 +2526,7 @@
         <c:axId val="1574855759"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4.5000000000000014E-3"/>
+          <c:max val="8.0000000000000019E-3"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2502,7 +2545,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.0000_ " sourceLinked="0"/>
+        <c:numFmt formatCode="0.000_ " sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2536,7 +2579,6 @@
         <c:crossAx val="1574853679"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="5.0000000000000012E-4"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3186,13 +3228,13 @@
                 <c:formatCode>0.000000_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.3380910146342928</c:v>
+                  <c:v>1.4310873022771393</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2350004372139893</c:v>
+                  <c:v>0.99787591008393206</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.88139292853091633</c:v>
+                  <c:v>0.79509818044537628</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3266,13 +3308,13 @@
                 <c:formatCode>0.000000_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.8070178652893787</c:v>
+                  <c:v>1.3705475197567627</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1966565253799044</c:v>
+                  <c:v>1.008633402328275</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0424281172443055</c:v>
+                  <c:v>0.92581916692649013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3352,6 +3394,8 @@
         <c:axId val="1312776351"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.5"/>
+          <c:min val="0.70000000000000007"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3703,22 +3747,22 @@
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40.138599999999997</c:v>
+                  <c:v>65.5779</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>72.0471</c:v>
+                  <c:v>89.167599999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90.801500000000004</c:v>
+                  <c:v>100.65649999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54.5807</c:v>
+                  <c:v>71.962699999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76.190200000000004</c:v>
+                  <c:v>90.393100000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>86.025499999999994</c:v>
+                  <c:v>96.860600000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3797,8 +3841,8 @@
         <c:axId val="1679869296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100"/>
-          <c:min val="30"/>
+          <c:max val="105"/>
+          <c:min val="65"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -8209,8 +8253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -8222,32 +8266,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="F1" s="26" t="s">
+      <c r="D1" s="33"/>
+      <c r="F1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="26"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="27"/>
+      <c r="F2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="21"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="24"/>
-      <c r="B3" s="25"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="1">
         <v>6</v>
       </c>
@@ -8262,7 +8306,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -8284,7 +8328,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="18"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -8304,7 +8348,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="18"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -8324,7 +8368,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="18"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -8344,7 +8388,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="18"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -8364,7 +8408,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="19"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -8384,32 +8428,32 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="F11" s="26" t="s">
+      <c r="D11" s="33"/>
+      <c r="F11" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="26"/>
+      <c r="G11" s="32"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="20" t="s">
+      <c r="B12" s="29"/>
+      <c r="C12" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="21"/>
-      <c r="F12" s="20" t="s">
+      <c r="D12" s="27"/>
+      <c r="F12" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="21"/>
+      <c r="G12" s="27"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="24"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="1">
         <v>6</v>
       </c>
@@ -8424,7 +8468,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -8446,7 +8490,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="18"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
@@ -8466,7 +8510,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="18"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
@@ -8486,7 +8530,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="18"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
@@ -8506,7 +8550,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="18"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
@@ -8526,7 +8570,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="19"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
@@ -8546,24 +8590,24 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F21" s="27" t="s">
+      <c r="F21" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="27"/>
+      <c r="G21" s="33"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="F22" s="20" t="s">
+      <c r="B22" s="29"/>
+      <c r="F22" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="21"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="24"/>
-      <c r="B23" s="25"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="31"/>
       <c r="F23" s="1">
         <v>6</v>
       </c>
@@ -8572,7 +8616,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -8586,7 +8630,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" s="18"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
@@ -8598,7 +8642,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="18"/>
+      <c r="A26" s="24"/>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
@@ -8610,7 +8654,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="18"/>
+      <c r="A27" s="24"/>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
@@ -8622,7 +8666,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A28" s="18"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
@@ -8634,7 +8678,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" s="19"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
@@ -8646,24 +8690,24 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F31" s="26" t="s">
+      <c r="F31" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="26"/>
+      <c r="G31" s="32"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="23"/>
-      <c r="F32" s="20" t="s">
+      <c r="B32" s="29"/>
+      <c r="F32" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="G32" s="21"/>
+      <c r="G32" s="27"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" s="24"/>
-      <c r="B33" s="25"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="31"/>
       <c r="F33" s="1">
         <v>6</v>
       </c>
@@ -8672,7 +8716,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -8688,7 +8732,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A35" s="18"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
@@ -8702,7 +8746,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A36" s="18"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="1" t="s">
         <v>4</v>
       </c>
@@ -8716,7 +8760,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="18"/>
+      <c r="A37" s="24"/>
       <c r="B37" s="1" t="s">
         <v>5</v>
       </c>
@@ -8730,7 +8774,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A38" s="18"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="1" t="s">
         <v>6</v>
       </c>
@@ -8744,7 +8788,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A39" s="19"/>
+      <c r="A39" s="25"/>
       <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
@@ -8788,47 +8832,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:B32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="9"/>
+    <col min="1" max="1" width="8.6640625" style="7"/>
     <col min="2" max="3" width="14.25" customWidth="1"/>
     <col min="4" max="7" width="11.58203125" customWidth="1"/>
-    <col min="8" max="11" width="8.6640625" style="9"/>
+    <col min="8" max="11" width="8.6640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="30" t="s">
+    <row r="1" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="28" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28" t="s">
+      <c r="E2" s="38"/>
+      <c r="F2" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="28"/>
+      <c r="G2" s="38"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B3" s="9"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="11" t="s">
         <v>27</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -8836,19 +8880,19 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="36" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="18">
         <v>93.847700000000003</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="19">
         <v>98.628299999999996</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="12">
         <f t="shared" ref="F4:G6" si="0">F16*D4/100</f>
         <v>1.0174967634E-2</v>
       </c>
@@ -8858,17 +8902,17 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B5" s="29"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="18">
         <v>88.978200000000001</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="19">
         <v>91.173500000000004</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="12">
         <f t="shared" si="0"/>
         <v>2.6257466820000003E-3</v>
       </c>
@@ -8878,17 +8922,17 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B6" s="29"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="18">
         <v>80.031800000000004</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="19">
         <v>89.675399999999996</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="12">
         <f t="shared" si="0"/>
         <v>7.9551609200000008E-4</v>
       </c>
@@ -8897,33 +8941,33 @@
         <v>5.2549784399999998E-4</v>
       </c>
     </row>
-    <row r="7" spans="2:7" s="9" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="8" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="30" t="s">
+    <row r="7" spans="2:7" s="7" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="8" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="28" t="s">
+      <c r="C8" s="39"/>
+      <c r="D8" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28" t="s">
+      <c r="E8" s="38"/>
+      <c r="F8" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="28"/>
+      <c r="G8" s="38"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B9" s="9"/>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="11" t="s">
         <v>27</v>
       </c>
       <c r="G9" s="5" t="s">
@@ -8931,83 +8975,83 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="36" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="6">
-        <v>40.138599999999997</v>
-      </c>
-      <c r="E10" s="16">
-        <v>54.5807</v>
-      </c>
-      <c r="F10" s="14">
+      <c r="D10" s="21">
+        <v>65.5779</v>
+      </c>
+      <c r="E10" s="22">
+        <v>71.962699999999998</v>
+      </c>
+      <c r="F10" s="12">
         <f t="shared" ref="F10:G12" si="1">F16*D10/100</f>
-        <v>4.351827011999999E-3</v>
+        <v>7.1099559179999992E-3</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="1"/>
-        <v>3.7393237570000006E-3</v>
+        <v>4.9301645770000006E-3</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B11" s="29"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="6">
-        <v>72.0471</v>
-      </c>
-      <c r="E11" s="16">
-        <v>76.190200000000004</v>
-      </c>
-      <c r="F11" s="14">
+      <c r="D11" s="21">
+        <v>89.167599999999993</v>
+      </c>
+      <c r="E11" s="22">
+        <v>90.393100000000004</v>
+      </c>
+      <c r="F11" s="12">
         <f t="shared" si="1"/>
-        <v>2.1261099209999999E-3</v>
+        <v>2.6313358759999998E-3</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="1"/>
-        <v>1.3630426780000002E-3</v>
+        <v>1.6171325590000002E-3</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B12" s="29"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="6">
-        <v>90.801500000000004</v>
-      </c>
-      <c r="E12" s="16">
-        <v>86.025499999999994</v>
-      </c>
-      <c r="F12" s="14">
+      <c r="D12" s="21">
+        <v>100.65649999999999</v>
+      </c>
+      <c r="E12" s="22">
+        <v>96.860600000000005</v>
+      </c>
+      <c r="F12" s="12">
         <f t="shared" si="1"/>
-        <v>9.025669100000001E-4</v>
+        <v>1.0005256099999999E-3</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="1"/>
-        <v>5.0410943E-4</v>
+        <v>5.6760311600000004E-4</v>
       </c>
     </row>
-    <row r="13" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="13" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="14" spans="2:7" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="31" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="31"/>
+      <c r="G14" s="37"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="7" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -9018,65 +9062,65 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="29" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="36" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="20">
         <v>1.0841999999999999E-2</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="20">
         <v>6.8510000000000003E-3</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="29"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="36"/>
       <c r="E17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="20">
         <v>2.9510000000000001E-3</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="20">
         <v>1.789E-3</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="29"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="36"/>
       <c r="E18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="20">
         <v>9.9400000000000009E-4</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="20">
         <v>5.8600000000000004E-4</v>
       </c>
     </row>
-    <row r="19" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="19" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="20" spans="2:7" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="28" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="28"/>
+      <c r="G20" s="38"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="7" t="s">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -9087,9 +9131,9 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="29" t="s">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="36" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -9097,181 +9141,615 @@
       </c>
       <c r="F22" s="4">
         <f t="shared" ref="F22:G24" si="2">F4/F10</f>
-        <v>2.3380910146342928</v>
+        <v>1.4310873022771393</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="2"/>
-        <v>1.8070178652893787</v>
+        <v>1.3705475197567627</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="29"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="36"/>
       <c r="E23" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F23" s="4">
         <f t="shared" si="2"/>
-        <v>1.2350004372139893</v>
+        <v>0.99787591008393206</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" si="2"/>
-        <v>1.1966565253799044</v>
+        <v>1.008633402328275</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="29"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="36"/>
       <c r="E24" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F24" s="4">
         <f t="shared" si="2"/>
-        <v>0.88139292853091633</v>
+        <v>0.79509818044537628</v>
       </c>
       <c r="G24" s="4">
         <f t="shared" si="2"/>
-        <v>1.0424281172443055</v>
+        <v>0.92581916692649013</v>
       </c>
     </row>
-    <row r="25" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="26" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="C26" s="35" t="s">
+    <row r="25" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C26" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="33" t="s">
+      <c r="E26" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="2:7" s="9" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="36" t="s">
+    <row r="27" spans="2:7" s="7" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="33" t="s">
+      <c r="C27" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="34">
+      <c r="D27" s="16">
         <f>D4</f>
         <v>93.847700000000003</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="16">
         <f>D10</f>
-        <v>40.138599999999997</v>
+        <v>65.5779</v>
       </c>
     </row>
-    <row r="28" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="37"/>
-      <c r="C28" s="33" t="s">
+    <row r="28" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B28" s="35"/>
+      <c r="C28" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="34">
+      <c r="D28" s="16">
         <f>D5</f>
         <v>88.978200000000001</v>
       </c>
-      <c r="E28" s="34">
+      <c r="E28" s="16">
         <f>D11</f>
-        <v>72.0471</v>
+        <v>89.167599999999993</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B29" s="37"/>
-      <c r="C29" s="33" t="s">
+      <c r="B29" s="35"/>
+      <c r="C29" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="34">
+      <c r="D29" s="16">
         <f>D6</f>
         <v>80.031800000000004</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="16">
         <f>D12</f>
-        <v>90.801500000000004</v>
+        <v>100.65649999999999</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B30" s="37"/>
-      <c r="C30" s="33" t="s">
+      <c r="B30" s="35"/>
+      <c r="C30" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="34">
+      <c r="D30" s="16">
         <f>E4</f>
         <v>98.628299999999996</v>
       </c>
-      <c r="E30" s="34">
+      <c r="E30" s="16">
         <f>E10</f>
-        <v>54.5807</v>
-      </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
+        <v>71.962699999999998</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B31" s="37"/>
-      <c r="C31" s="33" t="s">
+      <c r="B31" s="35"/>
+      <c r="C31" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="34">
+      <c r="D31" s="16">
         <f>E5</f>
         <v>91.173500000000004</v>
       </c>
-      <c r="E31" s="34">
+      <c r="E31" s="16">
         <f>E11</f>
-        <v>76.190200000000004</v>
-      </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
+        <v>90.393100000000004</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B32" s="37"/>
-      <c r="C32" s="33" t="s">
+      <c r="B32" s="35"/>
+      <c r="C32" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="34">
+      <c r="D32" s="16">
         <f>E6</f>
         <v>89.675399999999996</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="16">
         <f>E12</f>
-        <v>86.025499999999994</v>
-      </c>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
+        <v>96.860600000000005</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B48" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="39"/>
+      <c r="D48" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" s="38"/>
+      <c r="F48" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="38"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B49" s="7"/>
+      <c r="C49" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B50" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="41">
+        <f>D4</f>
+        <v>93.847700000000003</v>
+      </c>
+      <c r="E50" s="42">
+        <f t="shared" ref="E50:G50" si="3">E4</f>
+        <v>98.628299999999996</v>
+      </c>
+      <c r="F50" s="12">
+        <f t="shared" si="3"/>
+        <v>1.0174967634E-2</v>
+      </c>
+      <c r="G50" s="4">
+        <f t="shared" si="3"/>
+        <v>6.7570248330000001E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B51" s="36"/>
+      <c r="C51" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="41">
+        <f t="shared" ref="D51:G51" si="4">D5</f>
+        <v>88.978200000000001</v>
+      </c>
+      <c r="E51" s="42">
+        <f t="shared" si="4"/>
+        <v>91.173500000000004</v>
+      </c>
+      <c r="F51" s="12">
+        <f t="shared" si="4"/>
+        <v>2.6257466820000003E-3</v>
+      </c>
+      <c r="G51" s="4">
+        <f t="shared" si="4"/>
+        <v>1.6310939150000002E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B52" s="36"/>
+      <c r="C52" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="41">
+        <f t="shared" ref="D52:G52" si="5">D6</f>
+        <v>80.031800000000004</v>
+      </c>
+      <c r="E52" s="42">
+        <f t="shared" si="5"/>
+        <v>89.675399999999996</v>
+      </c>
+      <c r="F52" s="12">
+        <f t="shared" si="5"/>
+        <v>7.9551609200000008E-4</v>
+      </c>
+      <c r="G52" s="4">
+        <f t="shared" si="5"/>
+        <v>5.2549784399999998E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B54" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="39"/>
+      <c r="D54" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54" s="38"/>
+      <c r="F54" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" s="38"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B55" s="7"/>
+      <c r="C55" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B56" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" s="43">
+        <f t="shared" ref="D56:G56" si="6">D10</f>
+        <v>65.5779</v>
+      </c>
+      <c r="E56" s="44">
+        <f t="shared" si="6"/>
+        <v>71.962699999999998</v>
+      </c>
+      <c r="F56" s="12">
+        <f t="shared" si="6"/>
+        <v>7.1099559179999992E-3</v>
+      </c>
+      <c r="G56" s="4">
+        <f t="shared" si="6"/>
+        <v>4.9301645770000006E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B57" s="36"/>
+      <c r="C57" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D57" s="43">
+        <f t="shared" ref="D57:G57" si="7">D11</f>
+        <v>89.167599999999993</v>
+      </c>
+      <c r="E57" s="44">
+        <f t="shared" si="7"/>
+        <v>90.393100000000004</v>
+      </c>
+      <c r="F57" s="12">
+        <f t="shared" si="7"/>
+        <v>2.6313358759999998E-3</v>
+      </c>
+      <c r="G57" s="4">
+        <f t="shared" si="7"/>
+        <v>1.6171325590000002E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B58" s="36"/>
+      <c r="C58" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" s="43">
+        <f t="shared" ref="D58:G58" si="8">D12</f>
+        <v>100.65649999999999</v>
+      </c>
+      <c r="E58" s="44">
+        <f t="shared" si="8"/>
+        <v>96.860600000000005</v>
+      </c>
+      <c r="F58" s="12">
+        <f t="shared" si="8"/>
+        <v>1.0005256099999999E-3</v>
+      </c>
+      <c r="G58" s="4">
+        <f t="shared" si="8"/>
+        <v>5.6760311600000004E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="G60" s="37"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F62" s="40">
+        <f t="shared" ref="F62:G62" si="9">F16</f>
+        <v>1.0841999999999999E-2</v>
+      </c>
+      <c r="G62" s="40">
+        <f t="shared" si="9"/>
+        <v>6.8510000000000003E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="36"/>
+      <c r="E63" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F63" s="40">
+        <f t="shared" ref="F63:G63" si="10">F17</f>
+        <v>2.9510000000000001E-3</v>
+      </c>
+      <c r="G63" s="40">
+        <f t="shared" si="10"/>
+        <v>1.789E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F64" s="40">
+        <f t="shared" ref="F64:G64" si="11">F18</f>
+        <v>9.9400000000000009E-4</v>
+      </c>
+      <c r="G64" s="40">
+        <f t="shared" si="11"/>
+        <v>5.8600000000000004E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="G66" s="38"/>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F68" s="4">
+        <f t="shared" ref="F68:G68" si="12">F22</f>
+        <v>1.4310873022771393</v>
+      </c>
+      <c r="G68" s="4">
+        <f t="shared" si="12"/>
+        <v>1.3705475197567627</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="36"/>
+      <c r="E69" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F69" s="4">
+        <f t="shared" ref="F69:G69" si="13">F23</f>
+        <v>0.99787591008393206</v>
+      </c>
+      <c r="G69" s="4">
+        <f t="shared" si="13"/>
+        <v>1.008633402328275</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F70" s="4">
+        <f t="shared" ref="F70:G70" si="14">F24</f>
+        <v>0.79509818044537628</v>
+      </c>
+      <c r="G70" s="4">
+        <f t="shared" si="14"/>
+        <v>0.92581916692649013</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
+  <mergeCells count="25">
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="B4:B6"/>
@@ -9279,6 +9757,12 @@
     <mergeCell ref="D16:D18"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="J4:K6">

</xml_diff>

<commit_message>
add: revise the paper
</commit_message>
<xml_diff>
--- a/WPCN/for_final_paper.xlsx
+++ b/WPCN/for_final_paper.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="43">
   <si>
     <t>Problem/Size</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -412,6 +412,26 @@
     <t>16x16 / 10 WDs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>8x8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12x12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16x16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8x8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16x16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -753,7 +773,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -823,55 +843,7 @@
     <xf numFmtId="177" fontId="13" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -888,6 +860,57 @@
     </xf>
     <xf numFmtId="177" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3920,6 +3943,453 @@
         <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>CT.RATE (%) of our method vs. the methodology in original paper</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="ko-KR" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'for paper'!$N$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Our Method</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'for paper'!$M$50:$M$55</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8x8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12x12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16x16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8x8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12x12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16x16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'for paper'!$N$50:$N$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000_ </c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>93.847700000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>88.978200000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80.031800000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98.628299999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.173500000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89.675399999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-357A-418A-8EE7-94213F115CDF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'for paper'!$O$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Original Paper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'for paper'!$M$50:$M$55</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8x8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12x12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16x16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8x8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12x12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16x16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'for paper'!$O$50:$O$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000_ </c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>65.5779</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89.167599999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.65649999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>71.962699999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.393100000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.860600000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-357A-418A-8EE7-94213F115CDF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1222663904"/>
+        <c:axId val="1222663072"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1222663904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1222663072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1222663072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="65"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0_ " sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1222663904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4252,6 +4722,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -7271,6 +7781,509 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7985,6 +8998,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>488950</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8266,32 +9309,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="F1" s="32" t="s">
+      <c r="D1" s="36"/>
+      <c r="F1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="32"/>
+      <c r="G1" s="37"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="F2" s="26" t="s">
+      <c r="D2" s="39"/>
+      <c r="F2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="27"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="1">
         <v>6</v>
       </c>
@@ -8306,7 +9349,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -8328,7 +9371,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="24"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -8348,7 +9391,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="24"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -8368,7 +9411,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="24"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -8388,7 +9431,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="24"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -8408,7 +9451,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="25"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -8428,32 +9471,32 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="F11" s="32" t="s">
+      <c r="D11" s="36"/>
+      <c r="F11" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="32"/>
+      <c r="G11" s="37"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="26" t="s">
+      <c r="B12" s="33"/>
+      <c r="C12" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="F12" s="26" t="s">
+      <c r="D12" s="39"/>
+      <c r="F12" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="27"/>
+      <c r="G12" s="39"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="1">
         <v>6</v>
       </c>
@@ -8468,7 +9511,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -8490,7 +9533,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="24"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
@@ -8510,7 +9553,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="24"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
@@ -8530,7 +9573,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="24"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
@@ -8550,7 +9593,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="24"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
@@ -8570,7 +9613,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="25"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
@@ -8590,24 +9633,24 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="33"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="F22" s="26" t="s">
+      <c r="B22" s="33"/>
+      <c r="F22" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="27"/>
+      <c r="G22" s="39"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="30"/>
-      <c r="B23" s="31"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="35"/>
       <c r="F23" s="1">
         <v>6</v>
       </c>
@@ -8616,7 +9659,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -8630,7 +9673,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" s="24"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
@@ -8642,7 +9685,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="24"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
@@ -8654,7 +9697,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="24"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
@@ -8666,7 +9709,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A28" s="24"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
@@ -8678,7 +9721,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" s="25"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
@@ -8690,24 +9733,24 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F31" s="32" t="s">
+      <c r="F31" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="32"/>
+      <c r="G31" s="37"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="29"/>
-      <c r="F32" s="26" t="s">
+      <c r="B32" s="33"/>
+      <c r="F32" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G32" s="27"/>
+      <c r="G32" s="39"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" s="30"/>
-      <c r="B33" s="31"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="35"/>
       <c r="F33" s="1">
         <v>6</v>
       </c>
@@ -8716,7 +9759,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -8732,7 +9775,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A35" s="24"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
@@ -8746,7 +9789,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A36" s="24"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="1" t="s">
         <v>4</v>
       </c>
@@ -8760,7 +9803,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="24"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="1" t="s">
         <v>5</v>
       </c>
@@ -8774,7 +9817,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A38" s="24"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="1" t="s">
         <v>6</v>
       </c>
@@ -8788,7 +9831,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A39" s="25"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
@@ -8803,6 +9846,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A32:B33"/>
     <mergeCell ref="A34:A39"/>
     <mergeCell ref="A22:B23"/>
     <mergeCell ref="A24:A29"/>
@@ -8819,10 +9866,6 @@
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="A32:B33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8832,10 +9875,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K76"/>
+  <dimension ref="A1:S76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="C47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -8848,18 +9891,18 @@
   <sheetData>
     <row r="1" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="38" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38" t="s">
+      <c r="E2" s="42"/>
+      <c r="F2" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="38"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" s="7"/>
@@ -8880,7 +9923,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="40" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -8902,7 +9945,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B5" s="36"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
@@ -8922,7 +9965,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B6" s="36"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
@@ -8943,18 +9986,18 @@
     </row>
     <row r="7" spans="2:7" s="7" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="8" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="38" t="s">
+      <c r="C8" s="43"/>
+      <c r="D8" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38" t="s">
+      <c r="E8" s="42"/>
+      <c r="F8" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="38"/>
+      <c r="G8" s="42"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B9" s="7"/>
@@ -8975,7 +10018,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="40" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -8997,7 +10040,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B11" s="36"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
@@ -9017,7 +10060,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B12" s="36"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="5" t="s">
         <v>21</v>
       </c>
@@ -9042,10 +10085,10 @@
       <c r="C14" s="7"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="37" t="s">
+      <c r="F14" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="37"/>
+      <c r="G14" s="41"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B15" s="7"/>
@@ -9064,7 +10107,7 @@
     <row r="16" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="40" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -9080,7 +10123,7 @@
     <row r="17" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="36"/>
+      <c r="D17" s="40"/>
       <c r="E17" s="5" t="s">
         <v>20</v>
       </c>
@@ -9094,7 +10137,7 @@
     <row r="18" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="36"/>
+      <c r="D18" s="40"/>
       <c r="E18" s="5" t="s">
         <v>21</v>
       </c>
@@ -9111,10 +10154,10 @@
       <c r="C20" s="7"/>
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="38" t="s">
+      <c r="F20" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="38"/>
+      <c r="G20" s="42"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B21" s="7"/>
@@ -9133,7 +10176,7 @@
     <row r="22" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="40" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -9151,7 +10194,7 @@
     <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="36"/>
+      <c r="D23" s="40"/>
       <c r="E23" s="5" t="s">
         <v>20</v>
       </c>
@@ -9167,7 +10210,7 @@
     <row r="24" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="36"/>
+      <c r="D24" s="40"/>
       <c r="E24" s="5" t="s">
         <v>21</v>
       </c>
@@ -9193,7 +10236,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" s="7" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="44" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="15" t="s">
@@ -9209,7 +10252,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="35"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="15" t="s">
         <v>33</v>
       </c>
@@ -9223,7 +10266,7 @@
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B29" s="35"/>
+      <c r="B29" s="45"/>
       <c r="C29" s="15" t="s">
         <v>34</v>
       </c>
@@ -9237,7 +10280,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B30" s="35"/>
+      <c r="B30" s="45"/>
       <c r="C30" s="15" t="s">
         <v>35</v>
       </c>
@@ -9253,7 +10296,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B31" s="35"/>
+      <c r="B31" s="45"/>
       <c r="C31" s="15" t="s">
         <v>36</v>
       </c>
@@ -9269,7 +10312,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B32" s="35"/>
+      <c r="B32" s="45"/>
       <c r="C32" s="15" t="s">
         <v>37</v>
       </c>
@@ -9284,7 +10327,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -9292,7 +10335,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -9300,7 +10343,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -9308,29 +10351,45 @@
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="7"/>
+      <c r="S47" s="7"/>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B48" s="39" t="s">
+    <row r="48" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B48" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="39"/>
-      <c r="D48" s="38" t="s">
+      <c r="C48" s="43"/>
+      <c r="D48" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38" t="s">
+      <c r="E48" s="42"/>
+      <c r="F48" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="G48" s="38"/>
+      <c r="G48" s="42"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7"/>
+      <c r="S48" s="7"/>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:19" ht="17" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49" s="7"/>
       <c r="C49" s="6" t="s">
         <v>29</v>
@@ -9347,19 +10406,33 @@
       <c r="G49" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="L49" s="7"/>
+      <c r="M49" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="N49" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="O49" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="P49" s="7"/>
+      <c r="Q49" s="7"/>
+      <c r="R49" s="7"/>
+      <c r="S49" s="7"/>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B50" s="36" t="s">
+    <row r="50" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B50" s="40" t="s">
         <v>18</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D50" s="41">
+      <c r="D50" s="25">
         <f>D4</f>
         <v>93.847700000000003</v>
       </c>
-      <c r="E50" s="42">
+      <c r="E50" s="26">
         <f t="shared" ref="E50:G50" si="3">E4</f>
         <v>98.628299999999996</v>
       </c>
@@ -9371,74 +10444,156 @@
         <f t="shared" si="3"/>
         <v>6.7570248330000001E-3</v>
       </c>
+      <c r="L50" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="M50" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N50" s="16">
+        <f>D27</f>
+        <v>93.847700000000003</v>
+      </c>
+      <c r="O50" s="16">
+        <f t="shared" ref="O50:O55" si="4">E27</f>
+        <v>65.5779</v>
+      </c>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+      <c r="S50" s="7"/>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B51" s="36"/>
+    <row r="51" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B51" s="40"/>
       <c r="C51" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D51" s="41">
-        <f t="shared" ref="D51:G51" si="4">D5</f>
+      <c r="D51" s="25">
+        <f t="shared" ref="D51:G51" si="5">D5</f>
         <v>88.978200000000001</v>
       </c>
-      <c r="E51" s="42">
+      <c r="E51" s="26">
+        <f t="shared" si="5"/>
+        <v>91.173500000000004</v>
+      </c>
+      <c r="F51" s="12">
+        <f t="shared" si="5"/>
+        <v>2.6257466820000003E-3</v>
+      </c>
+      <c r="G51" s="4">
+        <f t="shared" si="5"/>
+        <v>1.6310939150000002E-3</v>
+      </c>
+      <c r="L51" s="45"/>
+      <c r="M51" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N51" s="16">
+        <f t="shared" ref="N51:N55" si="6">D28</f>
+        <v>88.978200000000001</v>
+      </c>
+      <c r="O51" s="16">
         <f t="shared" si="4"/>
-        <v>91.173500000000004</v>
-      </c>
-      <c r="F51" s="12">
-        <f t="shared" si="4"/>
-        <v>2.6257466820000003E-3</v>
-      </c>
-      <c r="G51" s="4">
-        <f t="shared" si="4"/>
-        <v>1.6310939150000002E-3</v>
-      </c>
+        <v>89.167599999999993</v>
+      </c>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="7"/>
+      <c r="R51" s="7"/>
+      <c r="S51" s="7"/>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B52" s="36"/>
+    <row r="52" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B52" s="40"/>
       <c r="C52" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D52" s="41">
-        <f t="shared" ref="D52:G52" si="5">D6</f>
+      <c r="D52" s="25">
+        <f t="shared" ref="D52:G52" si="7">D6</f>
         <v>80.031800000000004</v>
       </c>
-      <c r="E52" s="42">
-        <f t="shared" si="5"/>
+      <c r="E52" s="26">
+        <f t="shared" si="7"/>
         <v>89.675399999999996</v>
       </c>
       <c r="F52" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.9551609200000008E-4</v>
       </c>
       <c r="G52" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.2549784399999998E-4</v>
       </c>
+      <c r="L52" s="45"/>
+      <c r="M52" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N52" s="16">
+        <f t="shared" si="6"/>
+        <v>80.031800000000004</v>
+      </c>
+      <c r="O52" s="16">
+        <f t="shared" si="4"/>
+        <v>100.65649999999999</v>
+      </c>
+      <c r="P52" s="7"/>
+      <c r="Q52" s="7"/>
+      <c r="R52" s="7"/>
+      <c r="S52" s="7"/>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
+      <c r="L53" s="45"/>
+      <c r="M53" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="N53" s="16">
+        <f t="shared" si="6"/>
+        <v>98.628299999999996</v>
+      </c>
+      <c r="O53" s="16">
+        <f t="shared" si="4"/>
+        <v>71.962699999999998</v>
+      </c>
+      <c r="P53" s="7"/>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="7"/>
+      <c r="S53" s="7"/>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B54" s="39" t="s">
+    <row r="54" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B54" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="39"/>
-      <c r="D54" s="38" t="s">
+      <c r="C54" s="43"/>
+      <c r="D54" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38" t="s">
+      <c r="E54" s="42"/>
+      <c r="F54" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="G54" s="38"/>
+      <c r="G54" s="42"/>
+      <c r="L54" s="45"/>
+      <c r="M54" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N54" s="16">
+        <f t="shared" si="6"/>
+        <v>91.173500000000004</v>
+      </c>
+      <c r="O54" s="16">
+        <f t="shared" si="4"/>
+        <v>90.393100000000004</v>
+      </c>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="7"/>
+      <c r="S54" s="7"/>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B55" s="7"/>
       <c r="C55" s="6" t="s">
         <v>29</v>
@@ -9455,94 +10610,150 @@
       <c r="G55" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="L55" s="45"/>
+      <c r="M55" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N55" s="16">
+        <f t="shared" si="6"/>
+        <v>89.675399999999996</v>
+      </c>
+      <c r="O55" s="16">
+        <f t="shared" si="4"/>
+        <v>96.860600000000005</v>
+      </c>
+      <c r="P55" s="7"/>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="7"/>
+      <c r="S55" s="7"/>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B56" s="36" t="s">
+    <row r="56" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B56" s="40" t="s">
         <v>18</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D56" s="43">
-        <f t="shared" ref="D56:G56" si="6">D10</f>
+      <c r="D56" s="27">
+        <f t="shared" ref="D56:G56" si="8">D10</f>
         <v>65.5779</v>
       </c>
-      <c r="E56" s="44">
-        <f t="shared" si="6"/>
+      <c r="E56" s="28">
+        <f t="shared" si="8"/>
         <v>71.962699999999998</v>
       </c>
       <c r="F56" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>7.1099559179999992E-3</v>
       </c>
       <c r="G56" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4.9301645770000006E-3</v>
       </c>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="7"/>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="7"/>
+      <c r="S56" s="7"/>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B57" s="36"/>
+    <row r="57" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B57" s="40"/>
       <c r="C57" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D57" s="43">
-        <f t="shared" ref="D57:G57" si="7">D11</f>
+      <c r="D57" s="27">
+        <f t="shared" ref="D57:G57" si="9">D11</f>
         <v>89.167599999999993</v>
       </c>
-      <c r="E57" s="44">
-        <f t="shared" si="7"/>
+      <c r="E57" s="28">
+        <f t="shared" si="9"/>
         <v>90.393100000000004</v>
       </c>
       <c r="F57" s="12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.6313358759999998E-3</v>
       </c>
       <c r="G57" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.6171325590000002E-3</v>
       </c>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="7"/>
+      <c r="P57" s="7"/>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="7"/>
+      <c r="S57" s="7"/>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B58" s="36"/>
+    <row r="58" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B58" s="40"/>
       <c r="C58" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D58" s="43">
-        <f t="shared" ref="D58:G58" si="8">D12</f>
+      <c r="D58" s="27">
+        <f t="shared" ref="D58:G58" si="10">D12</f>
         <v>100.65649999999999</v>
       </c>
-      <c r="E58" s="44">
-        <f t="shared" si="8"/>
+      <c r="E58" s="28">
+        <f t="shared" si="10"/>
         <v>96.860600000000005</v>
       </c>
       <c r="F58" s="12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0005256099999999E-3</v>
       </c>
       <c r="G58" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>5.6760311600000004E-4</v>
       </c>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
+      <c r="N58" s="7"/>
+      <c r="O58" s="7"/>
+      <c r="P58" s="7"/>
+      <c r="Q58" s="7"/>
+      <c r="R58" s="7"/>
+      <c r="S58" s="7"/>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="7"/>
+      <c r="P59" s="7"/>
+      <c r="Q59" s="7"/>
+      <c r="R59" s="7"/>
+      <c r="S59" s="7"/>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
-      <c r="F60" s="37" t="s">
+      <c r="F60" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="G60" s="37"/>
+      <c r="G60" s="41"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="7"/>
+      <c r="P60" s="7"/>
+      <c r="Q60" s="7"/>
+      <c r="R60" s="7"/>
+      <c r="S60" s="7"/>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="8"/>
@@ -9555,76 +10766,124 @@
       <c r="G61" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="L61" s="7"/>
+      <c r="M61" s="7"/>
+      <c r="N61" s="7"/>
+      <c r="O61" s="7"/>
+      <c r="P61" s="7"/>
+      <c r="Q61" s="7"/>
+      <c r="R61" s="7"/>
+      <c r="S61" s="7"/>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
-      <c r="D62" s="36" t="s">
+      <c r="D62" s="40" t="s">
         <v>18</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F62" s="40">
-        <f t="shared" ref="F62:G62" si="9">F16</f>
+      <c r="F62" s="24">
+        <f t="shared" ref="F62:G62" si="11">F16</f>
         <v>1.0841999999999999E-2</v>
       </c>
-      <c r="G62" s="40">
-        <f t="shared" si="9"/>
+      <c r="G62" s="24">
+        <f t="shared" si="11"/>
         <v>6.8510000000000003E-3</v>
       </c>
+      <c r="L62" s="7"/>
+      <c r="M62" s="7"/>
+      <c r="N62" s="7"/>
+      <c r="O62" s="7"/>
+      <c r="P62" s="7"/>
+      <c r="Q62" s="7"/>
+      <c r="R62" s="7"/>
+      <c r="S62" s="7"/>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
-      <c r="D63" s="36"/>
+      <c r="D63" s="40"/>
       <c r="E63" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F63" s="40">
-        <f t="shared" ref="F63:G63" si="10">F17</f>
+      <c r="F63" s="24">
+        <f t="shared" ref="F63:G63" si="12">F17</f>
         <v>2.9510000000000001E-3</v>
       </c>
-      <c r="G63" s="40">
-        <f t="shared" si="10"/>
+      <c r="G63" s="24">
+        <f t="shared" si="12"/>
         <v>1.789E-3</v>
       </c>
+      <c r="L63" s="7"/>
+      <c r="M63" s="7"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="7"/>
+      <c r="P63" s="7"/>
+      <c r="Q63" s="7"/>
+      <c r="R63" s="7"/>
+      <c r="S63" s="7"/>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
-      <c r="D64" s="36"/>
+      <c r="D64" s="40"/>
       <c r="E64" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F64" s="40">
-        <f t="shared" ref="F64:G64" si="11">F18</f>
+      <c r="F64" s="24">
+        <f t="shared" ref="F64:G64" si="13">F18</f>
         <v>9.9400000000000009E-4</v>
       </c>
-      <c r="G64" s="40">
-        <f t="shared" si="11"/>
+      <c r="G64" s="24">
+        <f t="shared" si="13"/>
         <v>5.8600000000000004E-4</v>
       </c>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="7"/>
+      <c r="P64" s="7"/>
+      <c r="Q64" s="7"/>
+      <c r="R64" s="7"/>
+      <c r="S64" s="7"/>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="7"/>
+      <c r="P65" s="7"/>
+      <c r="Q65" s="7"/>
+      <c r="R65" s="7"/>
+      <c r="S65" s="7"/>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="9"/>
       <c r="E66" s="10"/>
-      <c r="F66" s="38" t="s">
+      <c r="F66" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="G66" s="38"/>
+      <c r="G66" s="42"/>
+      <c r="L66" s="7"/>
+      <c r="M66" s="7"/>
+      <c r="N66" s="7"/>
+      <c r="O66" s="7"/>
+      <c r="P66" s="7"/>
+      <c r="Q66" s="7"/>
+      <c r="R66" s="7"/>
+      <c r="S66" s="7"/>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
@@ -9637,82 +10896,138 @@
       <c r="G67" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="L67" s="7"/>
+      <c r="M67" s="7"/>
+      <c r="N67" s="7"/>
+      <c r="O67" s="7"/>
+      <c r="P67" s="7"/>
+      <c r="Q67" s="7"/>
+      <c r="R67" s="7"/>
+      <c r="S67" s="7"/>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
-      <c r="D68" s="36" t="s">
+      <c r="D68" s="40" t="s">
         <v>18</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F68" s="4">
-        <f t="shared" ref="F68:G68" si="12">F22</f>
+        <f t="shared" ref="F68:G68" si="14">F22</f>
         <v>1.4310873022771393</v>
       </c>
       <c r="G68" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.3705475197567627</v>
       </c>
+      <c r="L68" s="7"/>
+      <c r="M68" s="7"/>
+      <c r="N68" s="7"/>
+      <c r="O68" s="7"/>
+      <c r="P68" s="7"/>
+      <c r="Q68" s="7"/>
+      <c r="R68" s="7"/>
+      <c r="S68" s="7"/>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
-      <c r="D69" s="36"/>
+      <c r="D69" s="40"/>
       <c r="E69" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F69" s="4">
-        <f t="shared" ref="F69:G69" si="13">F23</f>
+        <f t="shared" ref="F69:G69" si="15">F23</f>
         <v>0.99787591008393206</v>
       </c>
       <c r="G69" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.008633402328275</v>
       </c>
+      <c r="L69" s="7"/>
+      <c r="M69" s="7"/>
+      <c r="N69" s="7"/>
+      <c r="O69" s="7"/>
+      <c r="P69" s="7"/>
+      <c r="Q69" s="7"/>
+      <c r="R69" s="7"/>
+      <c r="S69" s="7"/>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
-      <c r="D70" s="36"/>
+      <c r="D70" s="40"/>
       <c r="E70" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F70" s="4">
-        <f t="shared" ref="F70:G70" si="14">F24</f>
+        <f t="shared" ref="F70:G70" si="16">F24</f>
         <v>0.79509818044537628</v>
       </c>
       <c r="G70" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.92581916692649013</v>
       </c>
+      <c r="L70" s="7"/>
+      <c r="M70" s="7"/>
+      <c r="N70" s="7"/>
+      <c r="O70" s="7"/>
+      <c r="P70" s="7"/>
+      <c r="Q70" s="7"/>
+      <c r="R70" s="7"/>
+      <c r="S70" s="7"/>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
+      <c r="N71" s="7"/>
+      <c r="O71" s="7"/>
+      <c r="P71" s="7"/>
+      <c r="Q71" s="7"/>
+      <c r="R71" s="7"/>
+      <c r="S71" s="7"/>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
+      <c r="L72" s="7"/>
+      <c r="M72" s="7"/>
+      <c r="N72" s="7"/>
+      <c r="O72" s="7"/>
+      <c r="P72" s="7"/>
+      <c r="Q72" s="7"/>
+      <c r="R72" s="7"/>
+      <c r="S72" s="7"/>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="7"/>
+      <c r="N73" s="7"/>
+      <c r="O73" s="7"/>
+      <c r="P73" s="7"/>
+      <c r="Q73" s="7"/>
+      <c r="R73" s="7"/>
+      <c r="S73" s="7"/>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
@@ -9720,7 +11035,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
@@ -9728,7 +11043,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
@@ -9737,12 +11052,21 @@
       <c r="G76" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="D62:D64"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="D68:D70"/>
+  <mergeCells count="26">
+    <mergeCell ref="L50:L55"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="D48:E48"/>
     <mergeCell ref="F48:G48"/>
@@ -9750,19 +11074,11 @@
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="F54:G54"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="D68:D70"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="J4:K6">

</xml_diff>

<commit_message>
modify: revise final paper
</commit_message>
<xml_diff>
--- a/WPCN/for_final_paper.xlsx
+++ b/WPCN/for_final_paper.xlsx
@@ -861,13 +861,10 @@
     <xf numFmtId="177" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -882,17 +879,26 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -904,12 +910,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1027,7 +1027,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1038,11 +1038,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1461,7 +1461,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1472,11 +1472,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1899,7 +1899,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1910,11 +1910,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2338,7 +2338,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2349,11 +2349,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2773,7 +2773,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2784,11 +2784,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -3206,7 +3206,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -3217,11 +3217,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -3646,7 +3646,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -4093,7 +4093,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -9309,32 +9309,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="F1" s="37" t="s">
+      <c r="D1" s="38"/>
+      <c r="F1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="37"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="38" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="F2" s="38" t="s">
+      <c r="D2" s="30"/>
+      <c r="F2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="39"/>
+      <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="34"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="1">
         <v>6</v>
       </c>
@@ -9349,7 +9349,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -9371,7 +9371,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="30"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -9391,7 +9391,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="30"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -9411,7 +9411,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="30"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -9431,7 +9431,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="30"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -9451,7 +9451,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="31"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -9471,32 +9471,32 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="F11" s="37" t="s">
+      <c r="D11" s="38"/>
+      <c r="F11" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="37"/>
+      <c r="G11" s="39"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="38" t="s">
+      <c r="B12" s="32"/>
+      <c r="C12" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="F12" s="38" t="s">
+      <c r="D12" s="30"/>
+      <c r="F12" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="39"/>
+      <c r="G12" s="30"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="34"/>
-      <c r="B13" s="35"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="1">
         <v>6</v>
       </c>
@@ -9511,7 +9511,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -9533,7 +9533,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="30"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
@@ -9553,7 +9553,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="30"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
@@ -9573,7 +9573,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="30"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
@@ -9593,7 +9593,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="30"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
@@ -9613,7 +9613,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="31"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
@@ -9633,24 +9633,24 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F21" s="36" t="s">
+      <c r="F21" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="36"/>
+      <c r="G21" s="38"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="F22" s="38" t="s">
+      <c r="B22" s="32"/>
+      <c r="F22" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="39"/>
+      <c r="G22" s="30"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="34"/>
-      <c r="B23" s="35"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="34"/>
       <c r="F23" s="1">
         <v>6</v>
       </c>
@@ -9659,7 +9659,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -9673,7 +9673,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" s="30"/>
+      <c r="A25" s="36"/>
       <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
@@ -9685,7 +9685,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="30"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
@@ -9697,7 +9697,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="30"/>
+      <c r="A27" s="36"/>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
@@ -9709,7 +9709,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A28" s="30"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
@@ -9721,7 +9721,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" s="31"/>
+      <c r="A29" s="37"/>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
@@ -9733,24 +9733,24 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F31" s="37" t="s">
+      <c r="F31" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="37"/>
+      <c r="G31" s="39"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="F32" s="38" t="s">
+      <c r="B32" s="32"/>
+      <c r="F32" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G32" s="39"/>
+      <c r="G32" s="30"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" s="34"/>
-      <c r="B33" s="35"/>
+      <c r="A33" s="33"/>
+      <c r="B33" s="34"/>
       <c r="F33" s="1">
         <v>6</v>
       </c>
@@ -9759,7 +9759,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -9775,7 +9775,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A35" s="30"/>
+      <c r="A35" s="36"/>
       <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
@@ -9789,7 +9789,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A36" s="30"/>
+      <c r="A36" s="36"/>
       <c r="B36" s="1" t="s">
         <v>4</v>
       </c>
@@ -9803,7 +9803,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="30"/>
+      <c r="A37" s="36"/>
       <c r="B37" s="1" t="s">
         <v>5</v>
       </c>
@@ -9817,7 +9817,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A38" s="30"/>
+      <c r="A38" s="36"/>
       <c r="B38" s="1" t="s">
         <v>6</v>
       </c>
@@ -9831,7 +9831,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A39" s="31"/>
+      <c r="A39" s="37"/>
       <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
@@ -9846,13 +9846,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="A32:B33"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="A22:B23"/>
-    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="C11:D11"/>
@@ -9861,11 +9859,13 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A32:B33"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="A24:A29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9877,8 +9877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" topLeftCell="E49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T51" sqref="T51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -9891,18 +9891,18 @@
   <sheetData>
     <row r="1" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="42" t="s">
+      <c r="C2" s="45"/>
+      <c r="D2" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42" t="s">
+      <c r="E2" s="44"/>
+      <c r="F2" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="42"/>
+      <c r="G2" s="44"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" s="7"/>
@@ -9923,7 +9923,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="42" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -9945,7 +9945,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B5" s="40"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
@@ -9965,7 +9965,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B6" s="40"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
@@ -9986,18 +9986,18 @@
     </row>
     <row r="7" spans="2:7" s="7" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="8" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="42" t="s">
+      <c r="C8" s="45"/>
+      <c r="D8" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42" t="s">
+      <c r="E8" s="44"/>
+      <c r="F8" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="42"/>
+      <c r="G8" s="44"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B9" s="7"/>
@@ -10018,7 +10018,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="42" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -10040,7 +10040,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B11" s="40"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
@@ -10060,7 +10060,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B12" s="40"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="5" t="s">
         <v>21</v>
       </c>
@@ -10085,10 +10085,10 @@
       <c r="C14" s="7"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="41" t="s">
+      <c r="F14" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="41"/>
+      <c r="G14" s="43"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B15" s="7"/>
@@ -10107,7 +10107,7 @@
     <row r="16" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="42" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -10123,7 +10123,7 @@
     <row r="17" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="40"/>
+      <c r="D17" s="42"/>
       <c r="E17" s="5" t="s">
         <v>20</v>
       </c>
@@ -10137,7 +10137,7 @@
     <row r="18" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="40"/>
+      <c r="D18" s="42"/>
       <c r="E18" s="5" t="s">
         <v>21</v>
       </c>
@@ -10154,10 +10154,10 @@
       <c r="C20" s="7"/>
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="42" t="s">
+      <c r="F20" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="42"/>
+      <c r="G20" s="44"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B21" s="7"/>
@@ -10176,7 +10176,7 @@
     <row r="22" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="42" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -10194,7 +10194,7 @@
     <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="40"/>
+      <c r="D23" s="42"/>
       <c r="E23" s="5" t="s">
         <v>20</v>
       </c>
@@ -10210,7 +10210,7 @@
     <row r="24" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="40"/>
+      <c r="D24" s="42"/>
       <c r="E24" s="5" t="s">
         <v>21</v>
       </c>
@@ -10236,7 +10236,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" s="7" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="40" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="15" t="s">
@@ -10252,7 +10252,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="45"/>
+      <c r="B28" s="41"/>
       <c r="C28" s="15" t="s">
         <v>33</v>
       </c>
@@ -10266,7 +10266,7 @@
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B29" s="45"/>
+      <c r="B29" s="41"/>
       <c r="C29" s="15" t="s">
         <v>34</v>
       </c>
@@ -10280,7 +10280,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B30" s="45"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="15" t="s">
         <v>35</v>
       </c>
@@ -10296,7 +10296,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B31" s="45"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="15" t="s">
         <v>36</v>
       </c>
@@ -10312,7 +10312,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B32" s="45"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="15" t="s">
         <v>37</v>
       </c>
@@ -10368,18 +10368,18 @@
       <c r="S47" s="7"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B48" s="43" t="s">
+      <c r="B48" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="43"/>
-      <c r="D48" s="42" t="s">
+      <c r="C48" s="45"/>
+      <c r="D48" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="42"/>
-      <c r="F48" s="42" t="s">
+      <c r="E48" s="44"/>
+      <c r="F48" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="G48" s="42"/>
+      <c r="G48" s="44"/>
       <c r="L48" s="7"/>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
@@ -10422,7 +10422,7 @@
       <c r="S49" s="7"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B50" s="40" t="s">
+      <c r="B50" s="42" t="s">
         <v>18</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -10444,7 +10444,7 @@
         <f t="shared" si="3"/>
         <v>6.7570248330000001E-3</v>
       </c>
-      <c r="L50" s="44" t="s">
+      <c r="L50" s="40" t="s">
         <v>18</v>
       </c>
       <c r="M50" s="15" t="s">
@@ -10464,7 +10464,7 @@
       <c r="S50" s="7"/>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B51" s="40"/>
+      <c r="B51" s="42"/>
       <c r="C51" s="5" t="s">
         <v>20</v>
       </c>
@@ -10484,7 +10484,7 @@
         <f t="shared" si="5"/>
         <v>1.6310939150000002E-3</v>
       </c>
-      <c r="L51" s="45"/>
+      <c r="L51" s="41"/>
       <c r="M51" s="15" t="s">
         <v>39</v>
       </c>
@@ -10502,7 +10502,7 @@
       <c r="S51" s="7"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B52" s="40"/>
+      <c r="B52" s="42"/>
       <c r="C52" s="5" t="s">
         <v>21</v>
       </c>
@@ -10522,7 +10522,7 @@
         <f t="shared" si="7"/>
         <v>5.2549784399999998E-4</v>
       </c>
-      <c r="L52" s="45"/>
+      <c r="L52" s="41"/>
       <c r="M52" s="15" t="s">
         <v>40</v>
       </c>
@@ -10546,7 +10546,7 @@
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
-      <c r="L53" s="45"/>
+      <c r="L53" s="41"/>
       <c r="M53" s="15" t="s">
         <v>41</v>
       </c>
@@ -10564,19 +10564,19 @@
       <c r="S53" s="7"/>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B54" s="43" t="s">
+      <c r="B54" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="43"/>
-      <c r="D54" s="42" t="s">
+      <c r="C54" s="45"/>
+      <c r="D54" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42" t="s">
+      <c r="E54" s="44"/>
+      <c r="F54" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="G54" s="42"/>
-      <c r="L54" s="45"/>
+      <c r="G54" s="44"/>
+      <c r="L54" s="41"/>
       <c r="M54" s="15" t="s">
         <v>20</v>
       </c>
@@ -10610,7 +10610,7 @@
       <c r="G55" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L55" s="45"/>
+      <c r="L55" s="41"/>
       <c r="M55" s="15" t="s">
         <v>42</v>
       </c>
@@ -10628,7 +10628,7 @@
       <c r="S55" s="7"/>
     </row>
     <row r="56" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B56" s="40" t="s">
+      <c r="B56" s="42" t="s">
         <v>18</v>
       </c>
       <c r="C56" s="5" t="s">
@@ -10660,7 +10660,7 @@
       <c r="S56" s="7"/>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B57" s="40"/>
+      <c r="B57" s="42"/>
       <c r="C57" s="5" t="s">
         <v>20</v>
       </c>
@@ -10690,7 +10690,7 @@
       <c r="S57" s="7"/>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B58" s="40"/>
+      <c r="B58" s="42"/>
       <c r="C58" s="5" t="s">
         <v>21</v>
       </c>
@@ -10740,10 +10740,10 @@
       <c r="C60" s="7"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
-      <c r="F60" s="41" t="s">
+      <c r="F60" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="G60" s="41"/>
+      <c r="G60" s="43"/>
       <c r="L60" s="7"/>
       <c r="M60" s="7"/>
       <c r="N60" s="7"/>
@@ -10778,7 +10778,7 @@
     <row r="62" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
-      <c r="D62" s="40" t="s">
+      <c r="D62" s="42" t="s">
         <v>18</v>
       </c>
       <c r="E62" s="5" t="s">
@@ -10804,7 +10804,7 @@
     <row r="63" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
-      <c r="D63" s="40"/>
+      <c r="D63" s="42"/>
       <c r="E63" s="5" t="s">
         <v>20</v>
       </c>
@@ -10828,7 +10828,7 @@
     <row r="64" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
-      <c r="D64" s="40"/>
+      <c r="D64" s="42"/>
       <c r="E64" s="5" t="s">
         <v>21</v>
       </c>
@@ -10870,10 +10870,10 @@
       <c r="C66" s="7"/>
       <c r="D66" s="9"/>
       <c r="E66" s="10"/>
-      <c r="F66" s="42" t="s">
+      <c r="F66" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="G66" s="42"/>
+      <c r="G66" s="44"/>
       <c r="L66" s="7"/>
       <c r="M66" s="7"/>
       <c r="N66" s="7"/>
@@ -10908,7 +10908,7 @@
     <row r="68" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
-      <c r="D68" s="40" t="s">
+      <c r="D68" s="42" t="s">
         <v>18</v>
       </c>
       <c r="E68" s="5" t="s">
@@ -10934,7 +10934,7 @@
     <row r="69" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
-      <c r="D69" s="40"/>
+      <c r="D69" s="42"/>
       <c r="E69" s="5" t="s">
         <v>20</v>
       </c>
@@ -10958,7 +10958,7 @@
     <row r="70" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
-      <c r="D70" s="40"/>
+      <c r="D70" s="42"/>
       <c r="E70" s="5" t="s">
         <v>21</v>
       </c>
@@ -11053,32 +11053,32 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="L50:L55"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="L50:L55"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F20:G20"/>
     <mergeCell ref="D16:D18"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
     <mergeCell ref="B50:B52"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="F54:G54"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="D62:D64"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="D68:D70"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="J4:K6">

</xml_diff>

<commit_message>
revise on 200728 (except for word file)
</commit_message>
<xml_diff>
--- a/WPCN/for_final_paper.xlsx
+++ b/WPCN/for_final_paper.xlsx
@@ -861,6 +861,15 @@
     <xf numFmtId="177" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -879,26 +888,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -910,6 +904,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -962,13 +962,16 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:rPr lang="en-US" altLang="ko-KR">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
               <a:t>CT.RATE (%) of our methodology</a:t>
             </a:r>
           </a:p>
@@ -995,9 +998,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -1219,9 +1222,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -1279,9 +1282,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -1322,9 +1325,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -1396,13 +1399,16 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:rPr lang="en-US" altLang="ko-KR">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
               <a:t>CT.AVERAGE of our methodology</a:t>
             </a:r>
           </a:p>
@@ -1429,9 +1435,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -1653,9 +1659,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -1712,9 +1718,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -1755,9 +1761,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -1829,20 +1835,29 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:rPr lang="en-US" altLang="ko-KR">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
               <a:t>CT.RATE (%) of methodology in original</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
+              <a:rPr lang="en-US" altLang="ko-KR" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
               <a:t> paper</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" altLang="ko-KR"/>
+            <a:endParaRPr lang="en-US" altLang="ko-KR">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1867,9 +1882,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -2091,9 +2106,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -2151,9 +2166,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -2194,9 +2209,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -2268,20 +2283,29 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:rPr lang="en-US" altLang="ko-KR">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
               <a:t>CT.AVERAGE</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
+              <a:rPr lang="en-US" altLang="ko-KR" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
               <a:t> of methodology in original paper</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" altLang="ko-KR"/>
+            <a:endParaRPr lang="en-US" altLang="ko-KR">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2306,9 +2330,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -2530,9 +2554,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -2591,9 +2615,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -2634,9 +2658,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -2708,13 +2732,16 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:rPr lang="en-US" altLang="ko-KR">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
               <a:t>CT.AVGMAX</a:t>
             </a:r>
           </a:p>
@@ -2741,9 +2768,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -2965,9 +2992,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -3024,9 +3051,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -3067,9 +3094,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -3141,13 +3168,16 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:rPr lang="en-US" altLang="ko-KR">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
               <a:t>PR</a:t>
             </a:r>
           </a:p>
@@ -3174,9 +3204,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -3398,9 +3428,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -3459,9 +3489,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -3502,9 +3532,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -3576,20 +3606,29 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:rPr lang="en-US" altLang="ko-KR">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
               <a:t>CT.RATE (%) of</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
+              <a:rPr lang="en-US" altLang="ko-KR" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
               <a:t> our method vs. the methodology in original paper</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" altLang="ko-KR"/>
+            <a:endParaRPr lang="en-US" altLang="ko-KR">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3614,9 +3653,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -3838,16 +3877,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -3899,16 +3938,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -3942,16 +3981,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -4023,19 +4062,23 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:rPr>
               <a:t>CT.RATE (%) of our method vs. the methodology in original paper</a:t>
             </a:r>
             <a:endParaRPr lang="ko-KR" altLang="ko-KR" sz="1400">
               <a:effectLst/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:endParaRPr>
           </a:p>
         </c:rich>
@@ -4061,9 +4104,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -4292,9 +4335,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -4352,9 +4395,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="ko-KR"/>
@@ -4396,9 +4439,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="ko-KR"/>
@@ -8857,7 +8900,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>243300</xdr:colOff>
+      <xdr:colOff>387350</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>117749</xdr:rowOff>
     </xdr:to>
@@ -8881,13 +8924,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>457199</xdr:colOff>
+      <xdr:colOff>457198</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>171448</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>154399</xdr:colOff>
+      <xdr:colOff>336549</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>149498</xdr:rowOff>
     </xdr:to>
@@ -9309,32 +9352,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="F1" s="39" t="s">
+      <c r="D1" s="39"/>
+      <c r="F1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="39"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="F2" s="29" t="s">
+      <c r="D2" s="33"/>
+      <c r="F2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="30"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="33"/>
-      <c r="B3" s="34"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="1">
         <v>6</v>
       </c>
@@ -9349,7 +9392,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -9371,7 +9414,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="36"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -9391,7 +9434,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="36"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -9411,7 +9454,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="36"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -9431,7 +9474,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="36"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -9451,7 +9494,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="37"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -9471,32 +9514,32 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="38"/>
-      <c r="F11" s="39" t="s">
+      <c r="D11" s="39"/>
+      <c r="F11" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="39"/>
+      <c r="G11" s="38"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="29" t="s">
+      <c r="B12" s="35"/>
+      <c r="C12" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="F12" s="29" t="s">
+      <c r="D12" s="33"/>
+      <c r="F12" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="30"/>
+      <c r="G12" s="33"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="33"/>
-      <c r="B13" s="34"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="1">
         <v>6</v>
       </c>
@@ -9511,7 +9554,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -9533,7 +9576,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="36"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
@@ -9553,7 +9596,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="36"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
@@ -9573,7 +9616,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="36"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
@@ -9593,7 +9636,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="36"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
@@ -9613,7 +9656,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="37"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
@@ -9633,24 +9676,24 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F21" s="38" t="s">
+      <c r="F21" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="38"/>
+      <c r="G21" s="39"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="F22" s="29" t="s">
+      <c r="B22" s="35"/>
+      <c r="F22" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="30"/>
+      <c r="G22" s="33"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="33"/>
-      <c r="B23" s="34"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="37"/>
       <c r="F23" s="1">
         <v>6</v>
       </c>
@@ -9659,7 +9702,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -9673,7 +9716,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" s="36"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
@@ -9685,7 +9728,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="36"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
@@ -9697,7 +9740,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="36"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
@@ -9709,7 +9752,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A28" s="36"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
@@ -9721,7 +9764,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" s="37"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
@@ -9733,24 +9776,24 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F31" s="39" t="s">
+      <c r="F31" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="39"/>
+      <c r="G31" s="38"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="F32" s="29" t="s">
+      <c r="B32" s="35"/>
+      <c r="F32" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="G32" s="30"/>
+      <c r="G32" s="33"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" s="33"/>
-      <c r="B33" s="34"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="37"/>
       <c r="F33" s="1">
         <v>6</v>
       </c>
@@ -9759,7 +9802,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -9775,7 +9818,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A35" s="36"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
@@ -9789,7 +9832,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A36" s="36"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="1" t="s">
         <v>4</v>
       </c>
@@ -9803,7 +9846,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A37" s="36"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="1" t="s">
         <v>5</v>
       </c>
@@ -9817,7 +9860,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A38" s="36"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="1" t="s">
         <v>6</v>
       </c>
@@ -9831,7 +9874,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A39" s="37"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
@@ -9846,11 +9889,9 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="A24:A29"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="C11:D11"/>
@@ -9859,13 +9900,15 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="A12:B13"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A32:B33"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="A22:B23"/>
-    <mergeCell ref="A24:A29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9877,8 +9920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T51" sqref="T51"/>
+    <sheetView tabSelected="1" topLeftCell="E55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P75" sqref="P75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -9891,18 +9934,18 @@
   <sheetData>
     <row r="1" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="44" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44" t="s">
+      <c r="E2" s="42"/>
+      <c r="F2" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="44"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" s="7"/>
@@ -9923,7 +9966,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="40" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -9945,7 +9988,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B5" s="42"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
@@ -9965,7 +10008,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B6" s="42"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
@@ -9986,18 +10029,18 @@
     </row>
     <row r="7" spans="2:7" s="7" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="8" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="44" t="s">
+      <c r="C8" s="43"/>
+      <c r="D8" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44" t="s">
+      <c r="E8" s="42"/>
+      <c r="F8" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="44"/>
+      <c r="G8" s="42"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B9" s="7"/>
@@ -10018,7 +10061,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="40" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -10040,7 +10083,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B11" s="42"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
@@ -10060,7 +10103,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B12" s="42"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="5" t="s">
         <v>21</v>
       </c>
@@ -10085,10 +10128,10 @@
       <c r="C14" s="7"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="43" t="s">
+      <c r="F14" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="43"/>
+      <c r="G14" s="41"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B15" s="7"/>
@@ -10107,7 +10150,7 @@
     <row r="16" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="40" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -10123,7 +10166,7 @@
     <row r="17" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="42"/>
+      <c r="D17" s="40"/>
       <c r="E17" s="5" t="s">
         <v>20</v>
       </c>
@@ -10137,7 +10180,7 @@
     <row r="18" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="42"/>
+      <c r="D18" s="40"/>
       <c r="E18" s="5" t="s">
         <v>21</v>
       </c>
@@ -10154,10 +10197,10 @@
       <c r="C20" s="7"/>
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="44" t="s">
+      <c r="F20" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="44"/>
+      <c r="G20" s="42"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B21" s="7"/>
@@ -10176,7 +10219,7 @@
     <row r="22" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="40" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -10194,7 +10237,7 @@
     <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="42"/>
+      <c r="D23" s="40"/>
       <c r="E23" s="5" t="s">
         <v>20</v>
       </c>
@@ -10210,7 +10253,7 @@
     <row r="24" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="42"/>
+      <c r="D24" s="40"/>
       <c r="E24" s="5" t="s">
         <v>21</v>
       </c>
@@ -10236,7 +10279,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" s="7" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="44" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="15" t="s">
@@ -10252,7 +10295,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="41"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="15" t="s">
         <v>33</v>
       </c>
@@ -10266,7 +10309,7 @@
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B29" s="41"/>
+      <c r="B29" s="45"/>
       <c r="C29" s="15" t="s">
         <v>34</v>
       </c>
@@ -10280,7 +10323,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B30" s="41"/>
+      <c r="B30" s="45"/>
       <c r="C30" s="15" t="s">
         <v>35</v>
       </c>
@@ -10296,7 +10339,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B31" s="41"/>
+      <c r="B31" s="45"/>
       <c r="C31" s="15" t="s">
         <v>36</v>
       </c>
@@ -10312,7 +10355,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B32" s="41"/>
+      <c r="B32" s="45"/>
       <c r="C32" s="15" t="s">
         <v>37</v>
       </c>
@@ -10368,18 +10411,18 @@
       <c r="S47" s="7"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B48" s="45" t="s">
+      <c r="B48" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="45"/>
-      <c r="D48" s="44" t="s">
+      <c r="C48" s="43"/>
+      <c r="D48" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="44"/>
-      <c r="F48" s="44" t="s">
+      <c r="E48" s="42"/>
+      <c r="F48" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="G48" s="44"/>
+      <c r="G48" s="42"/>
       <c r="L48" s="7"/>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
@@ -10422,7 +10465,7 @@
       <c r="S49" s="7"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B50" s="42" t="s">
+      <c r="B50" s="40" t="s">
         <v>18</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -10444,7 +10487,7 @@
         <f t="shared" si="3"/>
         <v>6.7570248330000001E-3</v>
       </c>
-      <c r="L50" s="40" t="s">
+      <c r="L50" s="44" t="s">
         <v>18</v>
       </c>
       <c r="M50" s="15" t="s">
@@ -10464,7 +10507,7 @@
       <c r="S50" s="7"/>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B51" s="42"/>
+      <c r="B51" s="40"/>
       <c r="C51" s="5" t="s">
         <v>20</v>
       </c>
@@ -10484,7 +10527,7 @@
         <f t="shared" si="5"/>
         <v>1.6310939150000002E-3</v>
       </c>
-      <c r="L51" s="41"/>
+      <c r="L51" s="45"/>
       <c r="M51" s="15" t="s">
         <v>39</v>
       </c>
@@ -10502,7 +10545,7 @@
       <c r="S51" s="7"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B52" s="42"/>
+      <c r="B52" s="40"/>
       <c r="C52" s="5" t="s">
         <v>21</v>
       </c>
@@ -10522,7 +10565,7 @@
         <f t="shared" si="7"/>
         <v>5.2549784399999998E-4</v>
       </c>
-      <c r="L52" s="41"/>
+      <c r="L52" s="45"/>
       <c r="M52" s="15" t="s">
         <v>40</v>
       </c>
@@ -10546,7 +10589,7 @@
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
-      <c r="L53" s="41"/>
+      <c r="L53" s="45"/>
       <c r="M53" s="15" t="s">
         <v>41</v>
       </c>
@@ -10564,19 +10607,19 @@
       <c r="S53" s="7"/>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B54" s="45" t="s">
+      <c r="B54" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="45"/>
-      <c r="D54" s="44" t="s">
+      <c r="C54" s="43"/>
+      <c r="D54" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="44"/>
-      <c r="F54" s="44" t="s">
+      <c r="E54" s="42"/>
+      <c r="F54" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="G54" s="44"/>
-      <c r="L54" s="41"/>
+      <c r="G54" s="42"/>
+      <c r="L54" s="45"/>
       <c r="M54" s="15" t="s">
         <v>20</v>
       </c>
@@ -10610,7 +10653,7 @@
       <c r="G55" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L55" s="41"/>
+      <c r="L55" s="45"/>
       <c r="M55" s="15" t="s">
         <v>42</v>
       </c>
@@ -10628,7 +10671,7 @@
       <c r="S55" s="7"/>
     </row>
     <row r="56" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B56" s="42" t="s">
+      <c r="B56" s="40" t="s">
         <v>18</v>
       </c>
       <c r="C56" s="5" t="s">
@@ -10660,7 +10703,7 @@
       <c r="S56" s="7"/>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B57" s="42"/>
+      <c r="B57" s="40"/>
       <c r="C57" s="5" t="s">
         <v>20</v>
       </c>
@@ -10690,7 +10733,7 @@
       <c r="S57" s="7"/>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B58" s="42"/>
+      <c r="B58" s="40"/>
       <c r="C58" s="5" t="s">
         <v>21</v>
       </c>
@@ -10740,10 +10783,10 @@
       <c r="C60" s="7"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
-      <c r="F60" s="43" t="s">
+      <c r="F60" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="G60" s="43"/>
+      <c r="G60" s="41"/>
       <c r="L60" s="7"/>
       <c r="M60" s="7"/>
       <c r="N60" s="7"/>
@@ -10778,7 +10821,7 @@
     <row r="62" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
-      <c r="D62" s="42" t="s">
+      <c r="D62" s="40" t="s">
         <v>18</v>
       </c>
       <c r="E62" s="5" t="s">
@@ -10804,7 +10847,7 @@
     <row r="63" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
-      <c r="D63" s="42"/>
+      <c r="D63" s="40"/>
       <c r="E63" s="5" t="s">
         <v>20</v>
       </c>
@@ -10828,7 +10871,7 @@
     <row r="64" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
-      <c r="D64" s="42"/>
+      <c r="D64" s="40"/>
       <c r="E64" s="5" t="s">
         <v>21</v>
       </c>
@@ -10870,10 +10913,10 @@
       <c r="C66" s="7"/>
       <c r="D66" s="9"/>
       <c r="E66" s="10"/>
-      <c r="F66" s="44" t="s">
+      <c r="F66" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="G66" s="44"/>
+      <c r="G66" s="42"/>
       <c r="L66" s="7"/>
       <c r="M66" s="7"/>
       <c r="N66" s="7"/>
@@ -10908,7 +10951,7 @@
     <row r="68" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
-      <c r="D68" s="42" t="s">
+      <c r="D68" s="40" t="s">
         <v>18</v>
       </c>
       <c r="E68" s="5" t="s">
@@ -10934,7 +10977,7 @@
     <row r="69" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
-      <c r="D69" s="42"/>
+      <c r="D69" s="40"/>
       <c r="E69" s="5" t="s">
         <v>20</v>
       </c>
@@ -10958,7 +11001,7 @@
     <row r="70" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
-      <c r="D70" s="42"/>
+      <c r="D70" s="40"/>
       <c r="E70" s="5" t="s">
         <v>21</v>
       </c>
@@ -11053,18 +11096,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="D62:D64"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="D68:D70"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="B4:B6"/>
@@ -11079,6 +11110,18 @@
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="F54:G54"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="D68:D70"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="J4:K6">

</xml_diff>

<commit_message>
modify: update as November experiment
</commit_message>
<xml_diff>
--- a/WPCN/for_final_paper.xlsx
+++ b/WPCN/for_final_paper.xlsx
@@ -870,12 +870,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -888,20 +882,23 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -911,6 +908,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1075,13 +1075,13 @@
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>93.847700000000003</c:v>
+                  <c:v>94.278700000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88.978200000000001</c:v>
+                  <c:v>86.935699999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80.031800000000004</c:v>
+                  <c:v>79.441999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1155,13 +1155,13 @@
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>98.628299999999996</c:v>
+                  <c:v>100.4858</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91.173500000000004</c:v>
+                  <c:v>92.131</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>89.675399999999996</c:v>
+                  <c:v>90.499099999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1512,13 +1512,13 @@
                 <c:formatCode>0.000000_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.0174967634E-2</c:v>
+                  <c:v>1.0221696653999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6257466820000003E-3</c:v>
+                  <c:v>2.5654725070000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.9551609200000008E-4</c:v>
+                  <c:v>7.8965348E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1592,13 +1592,13 @@
                 <c:formatCode>0.000000_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6.7570248330000001E-3</c:v>
+                  <c:v>6.8842821580000005E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6310939150000002E-3</c:v>
+                  <c:v>1.6482235900000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.2549784399999998E-4</c:v>
+                  <c:v>5.3032472600000001E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3281,13 +3281,13 @@
                 <c:formatCode>0.000000_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.4310873022771393</c:v>
+                  <c:v>1.4376596383842728</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99787591008393206</c:v>
+                  <c:v>0.97496960779475972</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.79509818044537628</c:v>
+                  <c:v>0.78923864827408075</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3361,13 +3361,13 @@
                 <c:formatCode>0.000000_ </c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.3705475197567627</c:v>
+                  <c:v>1.396359502909146</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.008633402328275</c:v>
+                  <c:v>1.0192260249952705</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.92581916692649013</c:v>
+                  <c:v>0.93432314067845956</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3726,22 +3726,22 @@
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>93.847700000000003</c:v>
+                  <c:v>94.278700000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88.978200000000001</c:v>
+                  <c:v>86.935699999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80.031800000000004</c:v>
+                  <c:v>79.441999999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98.628299999999996</c:v>
+                  <c:v>100.4858</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91.173500000000004</c:v>
+                  <c:v>92.131</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89.675399999999996</c:v>
+                  <c:v>90.499099999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4177,22 +4177,22 @@
                 <c:formatCode>0.0000_ </c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>93.847700000000003</c:v>
+                  <c:v>94.278700000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88.978200000000001</c:v>
+                  <c:v>86.935699999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80.031800000000004</c:v>
+                  <c:v>79.441999999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98.628299999999996</c:v>
+                  <c:v>100.4858</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91.173500000000004</c:v>
+                  <c:v>92.131</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89.675399999999996</c:v>
+                  <c:v>90.499099999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9352,32 +9352,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="F1" s="38" t="s">
+      <c r="D1" s="36"/>
+      <c r="F1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="38"/>
+      <c r="G1" s="37"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="32" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="F2" s="32" t="s">
+      <c r="D2" s="39"/>
+      <c r="F2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="33"/>
+      <c r="G2" s="39"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="1">
         <v>6</v>
       </c>
@@ -9514,32 +9514,32 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="F11" s="38" t="s">
+      <c r="D11" s="36"/>
+      <c r="F11" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="38"/>
+      <c r="G11" s="37"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="32" t="s">
+      <c r="B12" s="33"/>
+      <c r="C12" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="F12" s="32" t="s">
+      <c r="D12" s="39"/>
+      <c r="F12" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="33"/>
+      <c r="G12" s="39"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="36"/>
-      <c r="B13" s="37"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="1">
         <v>6</v>
       </c>
@@ -9676,24 +9676,24 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F21" s="39" t="s">
+      <c r="F21" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="39"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="F22" s="32" t="s">
+      <c r="B22" s="33"/>
+      <c r="F22" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="33"/>
+      <c r="G22" s="39"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="36"/>
-      <c r="B23" s="37"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="35"/>
       <c r="F23" s="1">
         <v>6</v>
       </c>
@@ -9776,24 +9776,24 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F31" s="38" t="s">
+      <c r="F31" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="38"/>
+      <c r="G31" s="37"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="35"/>
-      <c r="F32" s="32" t="s">
+      <c r="B32" s="33"/>
+      <c r="F32" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G32" s="33"/>
+      <c r="G32" s="39"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" s="36"/>
-      <c r="B33" s="37"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="35"/>
       <c r="F33" s="1">
         <v>6</v>
       </c>
@@ -9889,6 +9889,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A32:B33"/>
     <mergeCell ref="A34:A39"/>
     <mergeCell ref="A22:B23"/>
     <mergeCell ref="A24:A29"/>
@@ -9905,10 +9909,6 @@
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="A32:B33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9920,8 +9920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P75" sqref="P75"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -9934,18 +9934,18 @@
   <sheetData>
     <row r="1" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="42" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42" t="s">
+      <c r="E2" s="40"/>
+      <c r="F2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="42"/>
+      <c r="G2" s="40"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B3" s="7"/>
@@ -9966,81 +9966,81 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="41" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="18">
-        <v>93.847700000000003</v>
+        <v>94.278700000000001</v>
       </c>
       <c r="E4" s="19">
-        <v>98.628299999999996</v>
+        <v>100.4858</v>
       </c>
       <c r="F4" s="12">
         <f t="shared" ref="F4:G6" si="0">F16*D4/100</f>
-        <v>1.0174967634E-2</v>
+        <v>1.0221696653999999E-2</v>
       </c>
       <c r="G4" s="4">
         <f t="shared" si="0"/>
-        <v>6.7570248330000001E-3</v>
+        <v>6.8842821580000005E-3</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B5" s="40"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="18">
-        <v>88.978200000000001</v>
+        <v>86.935699999999997</v>
       </c>
       <c r="E5" s="19">
-        <v>91.173500000000004</v>
+        <v>92.131</v>
       </c>
       <c r="F5" s="12">
         <f t="shared" si="0"/>
-        <v>2.6257466820000003E-3</v>
+        <v>2.5654725070000002E-3</v>
       </c>
       <c r="G5" s="4">
         <f t="shared" si="0"/>
-        <v>1.6310939150000002E-3</v>
+        <v>1.6482235900000001E-3</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B6" s="40"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="18">
-        <v>80.031800000000004</v>
+        <v>79.441999999999993</v>
       </c>
       <c r="E6" s="19">
-        <v>89.675399999999996</v>
+        <v>90.499099999999999</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="0"/>
-        <v>7.9551609200000008E-4</v>
+        <v>7.8965348E-4</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="0"/>
-        <v>5.2549784399999998E-4</v>
+        <v>5.3032472600000001E-4</v>
       </c>
     </row>
     <row r="7" spans="2:7" s="7" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="8" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="42" t="s">
+      <c r="C8" s="42"/>
+      <c r="D8" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42" t="s">
+      <c r="E8" s="40"/>
+      <c r="F8" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="42"/>
+      <c r="G8" s="40"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B9" s="7"/>
@@ -10061,7 +10061,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="41" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -10083,7 +10083,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B11" s="40"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
@@ -10103,7 +10103,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B12" s="40"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="5" t="s">
         <v>21</v>
       </c>
@@ -10128,10 +10128,10 @@
       <c r="C14" s="7"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="41" t="s">
+      <c r="F14" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="41"/>
+      <c r="G14" s="45"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B15" s="7"/>
@@ -10150,7 +10150,7 @@
     <row r="16" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="41" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -10166,7 +10166,7 @@
     <row r="17" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="40"/>
+      <c r="D17" s="41"/>
       <c r="E17" s="5" t="s">
         <v>20</v>
       </c>
@@ -10180,7 +10180,7 @@
     <row r="18" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="40"/>
+      <c r="D18" s="41"/>
       <c r="E18" s="5" t="s">
         <v>21</v>
       </c>
@@ -10197,10 +10197,10 @@
       <c r="C20" s="7"/>
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="42" t="s">
+      <c r="F20" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="42"/>
+      <c r="G20" s="40"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B21" s="7"/>
@@ -10219,7 +10219,7 @@
     <row r="22" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="41" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -10227,43 +10227,43 @@
       </c>
       <c r="F22" s="4">
         <f t="shared" ref="F22:G24" si="2">F4/F10</f>
-        <v>1.4310873022771393</v>
+        <v>1.4376596383842728</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="2"/>
-        <v>1.3705475197567627</v>
+        <v>1.396359502909146</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="40"/>
+      <c r="D23" s="41"/>
       <c r="E23" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F23" s="4">
         <f t="shared" si="2"/>
-        <v>0.99787591008393206</v>
+        <v>0.97496960779475972</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" si="2"/>
-        <v>1.008633402328275</v>
+        <v>1.0192260249952705</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="40"/>
+      <c r="D24" s="41"/>
       <c r="E24" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F24" s="4">
         <f t="shared" si="2"/>
-        <v>0.79509818044537628</v>
+        <v>0.78923864827408075</v>
       </c>
       <c r="G24" s="4">
         <f t="shared" si="2"/>
-        <v>0.92581916692649013</v>
+        <v>0.93432314067845956</v>
       </c>
     </row>
     <row r="25" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45"/>
@@ -10279,7 +10279,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" s="7" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="43" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="15" t="s">
@@ -10287,7 +10287,7 @@
       </c>
       <c r="D27" s="16">
         <f>D4</f>
-        <v>93.847700000000003</v>
+        <v>94.278700000000001</v>
       </c>
       <c r="E27" s="16">
         <f>D10</f>
@@ -10295,13 +10295,13 @@
       </c>
     </row>
     <row r="28" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="45"/>
+      <c r="B28" s="44"/>
       <c r="C28" s="15" t="s">
         <v>33</v>
       </c>
       <c r="D28" s="16">
         <f>D5</f>
-        <v>88.978200000000001</v>
+        <v>86.935699999999997</v>
       </c>
       <c r="E28" s="16">
         <f>D11</f>
@@ -10309,13 +10309,13 @@
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B29" s="45"/>
+      <c r="B29" s="44"/>
       <c r="C29" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D29" s="16">
         <f>D6</f>
-        <v>80.031800000000004</v>
+        <v>79.441999999999993</v>
       </c>
       <c r="E29" s="16">
         <f>D12</f>
@@ -10323,13 +10323,13 @@
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B30" s="45"/>
+      <c r="B30" s="44"/>
       <c r="C30" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="16">
         <f>E4</f>
-        <v>98.628299999999996</v>
+        <v>100.4858</v>
       </c>
       <c r="E30" s="16">
         <f>E10</f>
@@ -10339,13 +10339,13 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B31" s="45"/>
+      <c r="B31" s="44"/>
       <c r="C31" s="15" t="s">
         <v>36</v>
       </c>
       <c r="D31" s="16">
         <f>E5</f>
-        <v>91.173500000000004</v>
+        <v>92.131</v>
       </c>
       <c r="E31" s="16">
         <f>E11</f>
@@ -10355,13 +10355,13 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B32" s="45"/>
+      <c r="B32" s="44"/>
       <c r="C32" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D32" s="16">
         <f>E6</f>
-        <v>89.675399999999996</v>
+        <v>90.499099999999999</v>
       </c>
       <c r="E32" s="16">
         <f>E12</f>
@@ -10411,18 +10411,18 @@
       <c r="S47" s="7"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B48" s="43" t="s">
+      <c r="B48" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="43"/>
-      <c r="D48" s="42" t="s">
+      <c r="C48" s="42"/>
+      <c r="D48" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="42"/>
-      <c r="F48" s="42" t="s">
+      <c r="E48" s="40"/>
+      <c r="F48" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G48" s="42"/>
+      <c r="G48" s="40"/>
       <c r="L48" s="7"/>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
@@ -10465,7 +10465,7 @@
       <c r="S49" s="7"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B50" s="40" t="s">
+      <c r="B50" s="41" t="s">
         <v>18</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -10473,21 +10473,21 @@
       </c>
       <c r="D50" s="25">
         <f>D4</f>
-        <v>93.847700000000003</v>
+        <v>94.278700000000001</v>
       </c>
       <c r="E50" s="26">
         <f t="shared" ref="E50:G50" si="3">E4</f>
-        <v>98.628299999999996</v>
+        <v>100.4858</v>
       </c>
       <c r="F50" s="12">
         <f t="shared" si="3"/>
-        <v>1.0174967634E-2</v>
+        <v>1.0221696653999999E-2</v>
       </c>
       <c r="G50" s="4">
         <f t="shared" si="3"/>
-        <v>6.7570248330000001E-3</v>
-      </c>
-      <c r="L50" s="44" t="s">
+        <v>6.8842821580000005E-3</v>
+      </c>
+      <c r="L50" s="43" t="s">
         <v>18</v>
       </c>
       <c r="M50" s="15" t="s">
@@ -10495,7 +10495,7 @@
       </c>
       <c r="N50" s="16">
         <f>D27</f>
-        <v>93.847700000000003</v>
+        <v>94.278700000000001</v>
       </c>
       <c r="O50" s="16">
         <f t="shared" ref="O50:O55" si="4">E27</f>
@@ -10507,33 +10507,33 @@
       <c r="S50" s="7"/>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B51" s="40"/>
+      <c r="B51" s="41"/>
       <c r="C51" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D51" s="25">
         <f t="shared" ref="D51:G51" si="5">D5</f>
-        <v>88.978200000000001</v>
+        <v>86.935699999999997</v>
       </c>
       <c r="E51" s="26">
         <f t="shared" si="5"/>
-        <v>91.173500000000004</v>
+        <v>92.131</v>
       </c>
       <c r="F51" s="12">
         <f t="shared" si="5"/>
-        <v>2.6257466820000003E-3</v>
+        <v>2.5654725070000002E-3</v>
       </c>
       <c r="G51" s="4">
         <f t="shared" si="5"/>
-        <v>1.6310939150000002E-3</v>
-      </c>
-      <c r="L51" s="45"/>
+        <v>1.6482235900000001E-3</v>
+      </c>
+      <c r="L51" s="44"/>
       <c r="M51" s="15" t="s">
         <v>39</v>
       </c>
       <c r="N51" s="16">
         <f t="shared" ref="N51:N55" si="6">D28</f>
-        <v>88.978200000000001</v>
+        <v>86.935699999999997</v>
       </c>
       <c r="O51" s="16">
         <f t="shared" si="4"/>
@@ -10545,33 +10545,33 @@
       <c r="S51" s="7"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B52" s="40"/>
+      <c r="B52" s="41"/>
       <c r="C52" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D52" s="25">
         <f t="shared" ref="D52:G52" si="7">D6</f>
-        <v>80.031800000000004</v>
+        <v>79.441999999999993</v>
       </c>
       <c r="E52" s="26">
         <f t="shared" si="7"/>
-        <v>89.675399999999996</v>
+        <v>90.499099999999999</v>
       </c>
       <c r="F52" s="12">
         <f t="shared" si="7"/>
-        <v>7.9551609200000008E-4</v>
+        <v>7.8965348E-4</v>
       </c>
       <c r="G52" s="4">
         <f t="shared" si="7"/>
-        <v>5.2549784399999998E-4</v>
-      </c>
-      <c r="L52" s="45"/>
+        <v>5.3032472600000001E-4</v>
+      </c>
+      <c r="L52" s="44"/>
       <c r="M52" s="15" t="s">
         <v>40</v>
       </c>
       <c r="N52" s="16">
         <f t="shared" si="6"/>
-        <v>80.031800000000004</v>
+        <v>79.441999999999993</v>
       </c>
       <c r="O52" s="16">
         <f t="shared" si="4"/>
@@ -10589,13 +10589,13 @@
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
-      <c r="L53" s="45"/>
+      <c r="L53" s="44"/>
       <c r="M53" s="15" t="s">
         <v>41</v>
       </c>
       <c r="N53" s="16">
         <f t="shared" si="6"/>
-        <v>98.628299999999996</v>
+        <v>100.4858</v>
       </c>
       <c r="O53" s="16">
         <f t="shared" si="4"/>
@@ -10607,25 +10607,25 @@
       <c r="S53" s="7"/>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B54" s="43" t="s">
+      <c r="B54" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="43"/>
-      <c r="D54" s="42" t="s">
+      <c r="C54" s="42"/>
+      <c r="D54" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42" t="s">
+      <c r="E54" s="40"/>
+      <c r="F54" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="G54" s="42"/>
-      <c r="L54" s="45"/>
+      <c r="G54" s="40"/>
+      <c r="L54" s="44"/>
       <c r="M54" s="15" t="s">
         <v>20</v>
       </c>
       <c r="N54" s="16">
         <f t="shared" si="6"/>
-        <v>91.173500000000004</v>
+        <v>92.131</v>
       </c>
       <c r="O54" s="16">
         <f t="shared" si="4"/>
@@ -10653,13 +10653,13 @@
       <c r="G55" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L55" s="45"/>
+      <c r="L55" s="44"/>
       <c r="M55" s="15" t="s">
         <v>42</v>
       </c>
       <c r="N55" s="16">
         <f t="shared" si="6"/>
-        <v>89.675399999999996</v>
+        <v>90.499099999999999</v>
       </c>
       <c r="O55" s="16">
         <f t="shared" si="4"/>
@@ -10671,7 +10671,7 @@
       <c r="S55" s="7"/>
     </row>
     <row r="56" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B56" s="40" t="s">
+      <c r="B56" s="41" t="s">
         <v>18</v>
       </c>
       <c r="C56" s="5" t="s">
@@ -10703,7 +10703,7 @@
       <c r="S56" s="7"/>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B57" s="40"/>
+      <c r="B57" s="41"/>
       <c r="C57" s="5" t="s">
         <v>20</v>
       </c>
@@ -10733,7 +10733,7 @@
       <c r="S57" s="7"/>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.45">
-      <c r="B58" s="40"/>
+      <c r="B58" s="41"/>
       <c r="C58" s="5" t="s">
         <v>21</v>
       </c>
@@ -10783,10 +10783,10 @@
       <c r="C60" s="7"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
-      <c r="F60" s="41" t="s">
+      <c r="F60" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="G60" s="41"/>
+      <c r="G60" s="45"/>
       <c r="L60" s="7"/>
       <c r="M60" s="7"/>
       <c r="N60" s="7"/>
@@ -10821,7 +10821,7 @@
     <row r="62" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
-      <c r="D62" s="40" t="s">
+      <c r="D62" s="41" t="s">
         <v>18</v>
       </c>
       <c r="E62" s="5" t="s">
@@ -10847,7 +10847,7 @@
     <row r="63" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
-      <c r="D63" s="40"/>
+      <c r="D63" s="41"/>
       <c r="E63" s="5" t="s">
         <v>20</v>
       </c>
@@ -10871,7 +10871,7 @@
     <row r="64" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
-      <c r="D64" s="40"/>
+      <c r="D64" s="41"/>
       <c r="E64" s="5" t="s">
         <v>21</v>
       </c>
@@ -10913,10 +10913,10 @@
       <c r="C66" s="7"/>
       <c r="D66" s="9"/>
       <c r="E66" s="10"/>
-      <c r="F66" s="42" t="s">
+      <c r="F66" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G66" s="42"/>
+      <c r="G66" s="40"/>
       <c r="L66" s="7"/>
       <c r="M66" s="7"/>
       <c r="N66" s="7"/>
@@ -10951,7 +10951,7 @@
     <row r="68" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
-      <c r="D68" s="40" t="s">
+      <c r="D68" s="41" t="s">
         <v>18</v>
       </c>
       <c r="E68" s="5" t="s">
@@ -10959,11 +10959,11 @@
       </c>
       <c r="F68" s="4">
         <f t="shared" ref="F68:G68" si="14">F22</f>
-        <v>1.4310873022771393</v>
+        <v>1.4376596383842728</v>
       </c>
       <c r="G68" s="4">
         <f t="shared" si="14"/>
-        <v>1.3705475197567627</v>
+        <v>1.396359502909146</v>
       </c>
       <c r="L68" s="7"/>
       <c r="M68" s="7"/>
@@ -10977,17 +10977,17 @@
     <row r="69" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
-      <c r="D69" s="40"/>
+      <c r="D69" s="41"/>
       <c r="E69" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F69" s="4">
         <f t="shared" ref="F69:G69" si="15">F23</f>
-        <v>0.99787591008393206</v>
+        <v>0.97496960779475972</v>
       </c>
       <c r="G69" s="4">
         <f t="shared" si="15"/>
-        <v>1.008633402328275</v>
+        <v>1.0192260249952705</v>
       </c>
       <c r="L69" s="7"/>
       <c r="M69" s="7"/>
@@ -11001,17 +11001,17 @@
     <row r="70" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
-      <c r="D70" s="40"/>
+      <c r="D70" s="41"/>
       <c r="E70" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F70" s="4">
         <f t="shared" ref="F70:G70" si="16">F24</f>
-        <v>0.79509818044537628</v>
+        <v>0.78923864827408075</v>
       </c>
       <c r="G70" s="4">
         <f t="shared" si="16"/>
-        <v>0.92581916692649013</v>
+        <v>0.93432314067845956</v>
       </c>
       <c r="L70" s="7"/>
       <c r="M70" s="7"/>
@@ -11096,6 +11096,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="B4:B6"/>
@@ -11112,16 +11122,6 @@
     <mergeCell ref="F54:G54"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="D62:D64"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="D68:D70"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="J4:K6">

</xml_diff>